<commit_message>
updated with summary tables
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EF44CB-D2BC-4682-BF13-C4976C5B6123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D9AF8F-182A-429F-A848-46F113D19991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
+    <sheet name="summary tables (Roman#)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="460">
   <si>
     <t>Countries</t>
   </si>
@@ -554,9 +555,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>COLUMNS</t>
-  </si>
-  <si>
     <t>Number of ordinations of diocesan priests</t>
   </si>
   <si>
@@ -587,18 +585,6 @@
     <t>Number of candidates for priesthood in the secondary-school centres (diocesan and religious)</t>
   </si>
   <si>
-    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 (TOTAL)</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 (INSTITUTA EX CONGREGATIONE PRO ECLESIIS ORIENTALIBUS PENDENTIA)</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 (INSTITUTA EX CONGREGATIONE PRO GENTIUM EVANGELIZATIONE PENDENTIA)</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 (INSTITUTA EX CONGREGATIONE PRO INSTITUTIS VITAE CONSACRATAE ET SOCIETATIBUS VITAE APOSTOLICAE PENDENTIA)</t>
-  </si>
-  <si>
     <t>Novices Seminarians</t>
   </si>
   <si>
@@ -608,12 +594,6 @@
     <t>Novices Total</t>
   </si>
   <si>
-    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 (TOTAL)</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 (INSTITUTA EX CONGREGATIONE PRO ECLESIIS ORIENTALIBUS PENDENTIA)</t>
-  </si>
-  <si>
     <t>Priests</t>
   </si>
   <si>
@@ -686,72 +666,9 @@
     <t>Lay people aw/i</t>
   </si>
   <si>
-    <t>Number of religious priests (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Number of religious priests (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of ordinations of religious priests (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 (INSTITUTA EX CONGREGATIONE PRO GENTIUM EVANGELIZATIONE PENDENTIA)</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 (INSTITUTA EX CONGREGATIONE PRO INSTITUTIS VITAE CONSACRATAE ET SOCIETATIBUS VITAE APOSTOLICAE PENDENTIA)</t>
-  </si>
-  <si>
     <t>Autonomous Houses</t>
   </si>
   <si>
-    <t>Number of ordinations of religious priests (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of defections of religious priests (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Number of defections of religious priests (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of deaths of religious priests (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Number of deaths of religious priests (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of non-priest men religious with temporary vows (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Number of non-priest men religious with temporary vows (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of non-priest men religious with perpetual vows (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Number of non-priest men religious with perpetual vows (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of seminarians (excluding novices) (ABSOLUTE FIGURES)</t>
-  </si>
-  <si>
-    <t>Number of seminarians (excluding novices) (INDEX NUMBERS (BASE 2013 = 100))</t>
-  </si>
-  <si>
-    <t>Number of novices in religious institutes for men (SEMINARIANS)</t>
-  </si>
-  <si>
-    <t>Number of novices in religious institutes for men (OTHERS)</t>
-  </si>
-  <si>
-    <t>Some significant data about papal-jurisdiction institutes for women (Autonomous Houses)</t>
-  </si>
-  <si>
-    <t>Some significant data about papal-jurisdiction institutes for women (Centralized Institutes)</t>
-  </si>
-  <si>
-    <t>Some significant data about papal-jurisdiction institutes for women (Secular Institutes)</t>
-  </si>
-  <si>
     <t>07. DIOCESAN AND REGIONAL TRIBUNALS</t>
   </si>
   <si>
@@ -881,60 +798,24 @@
     <t>Processes pres death tp</t>
   </si>
   <si>
-    <t>Area, population, ecclesiastical territories and centres on 31dec22</t>
-  </si>
-  <si>
-    <t>Ecclesiastical territories on 31dec22</t>
-  </si>
-  <si>
-    <t>Parishes with or without pastor on 31dec22</t>
-  </si>
-  <si>
     <t>Some statistical indices of ecclesiastical structure in 2022</t>
   </si>
   <si>
-    <t>Workforce for the Church's apostolate on 31dec22</t>
-  </si>
-  <si>
     <t>Some statistical indices of pastoral workload in 2022</t>
   </si>
   <si>
-    <t>Diocesan and titular bishops on 31dec22</t>
-  </si>
-  <si>
-    <t>Secular and religious episcopate, by rank, on 31dec22</t>
-  </si>
-  <si>
-    <t>Bishops, by main office held, on 31dec22</t>
-  </si>
-  <si>
-    <t>Diocesan priests, incardinated and present, on 31dec22</t>
-  </si>
-  <si>
     <t>Variations in the number of incardinated diocesan priests in 2022</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Ordinations, deaths, and defections of diocesan priests as percentages of those incardinated at boy22</t>
-  </si>
-  <si>
-    <t>Centres of formation for the priesthood on 31dec22</t>
-  </si>
-  <si>
-    <t>Candidates for the priesthood on 31dec22</t>
-  </si>
-  <si>
     <t>Some statistical indices of candidates for the priesthood (diocesan and religious) in 2022</t>
   </si>
   <si>
     <t>Candidates for the diocesan priesthood who left the seminary in 2022</t>
   </si>
   <si>
-    <t>Educational institutions on 31dec22</t>
-  </si>
-  <si>
     <t>Baptisms and marriages in 2022</t>
   </si>
   <si>
@@ -944,18 +825,6 @@
     <t>Baptisms of children up to 7yo and marriages. Rates per 1000 Catholics</t>
   </si>
   <si>
-    <t>Welfare institutions on 31dec22</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for men. Number of houses and of members on 31dec22</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for women: centralized institutes. Number of houses, novices, and professed religious on 31dec22</t>
-  </si>
-  <si>
-    <t>Papal-jurisdiction institutes for women: secular institutes. Number of candidates admitted to probation period, of members incorporated, and of lay people associated with the institute on 31dec22</t>
-  </si>
-  <si>
     <t>Movement of cases for declaration of nullity of marriage in 2022. Ordinary process</t>
   </si>
   <si>
@@ -981,13 +850,580 @@
   </si>
   <si>
     <t>Matrimonial processes according to the system for costs of processes in 2022</t>
+  </si>
+  <si>
+    <t>I-a</t>
+  </si>
+  <si>
+    <t>Estimates of population and Catholics in 2022</t>
+  </si>
+  <si>
+    <t>I-b</t>
+  </si>
+  <si>
+    <t>I-c</t>
+  </si>
+  <si>
+    <t>I-d</t>
+  </si>
+  <si>
+    <t>Average diocesan area (in km^2)</t>
+  </si>
+  <si>
+    <t>I-e</t>
+  </si>
+  <si>
+    <t>Pastoral centres by size on 31 December 2022</t>
+  </si>
+  <si>
+    <t>I-f</t>
+  </si>
+  <si>
+    <t>Pastoral density index (number of inhabitants per pastoral centre)</t>
+  </si>
+  <si>
+    <t>Pastoral centres by type on 31 December 2022</t>
+  </si>
+  <si>
+    <t>I-g</t>
+  </si>
+  <si>
+    <t>I-h</t>
+  </si>
+  <si>
+    <t>Number of pastoral centres - absolute figures</t>
+  </si>
+  <si>
+    <t>I-i</t>
+  </si>
+  <si>
+    <t>Number of parishes - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of parishes administered by a priest</t>
+  </si>
+  <si>
+    <t>Number of parishes entrusted to non-priests</t>
+  </si>
+  <si>
+    <t>Number of parishes completely vacant</t>
+  </si>
+  <si>
+    <t>Number of mission stations</t>
+  </si>
+  <si>
+    <t>I-l</t>
+  </si>
+  <si>
+    <t>I-m</t>
+  </si>
+  <si>
+    <t>I-n</t>
+  </si>
+  <si>
+    <t>I-o</t>
+  </si>
+  <si>
+    <t>I-p</t>
+  </si>
+  <si>
+    <t>Number of ecclesiastical territories - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of religious priests - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of religious priests - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of ordinations of religious priests - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of defections of religious priests - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of deaths of religious priests - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of non-priest men religious with temporary vows - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of non-priest men religious with perpetual vows - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of seminarians (excluding novices) - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of ordinations of religious priests - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of defections of religious priests - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of deaths of religious priests - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of seminarians (excluding novices) - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of non-priest men religious with perpetual vows - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of non-priest men religious with temporary vows - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of ecclesiastical territories - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of pastoral centres - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of parishes - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Area, population, ecclesiastical territories and centres on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Ecclesiastical territories on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Parishes with or without pastor on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Workforce for the Church's apostolate on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Diocesan and titular bishops on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Secular and religious episcopate, by rank, on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Bishops, by main office held, on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Diocesan priests, incardinated and present, on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Centres of formation for the priesthood on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Candidates for the priesthood on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Educational institutions on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Welfare institutions on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of houses and of members on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for women: centralized institutes. Number of houses, novices, and professed religious on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for women: secular institutes. Number of candidates admitted to probation period, of members incorporated, and of lay people associated with the institute on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Ecclesiastical territories on 31 December 2022, by rite</t>
+  </si>
+  <si>
+    <t>Ecclesiastical territories on 31 December 2022, by rank</t>
+  </si>
+  <si>
+    <t>Ecclesiastical territories not covered by the survey, by rank, on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Continents</t>
+  </si>
+  <si>
+    <t>Tot Pop (T)</t>
+  </si>
+  <si>
+    <t>Inh per km^2</t>
+  </si>
+  <si>
+    <t>Cath per 100 Ihn</t>
+  </si>
+  <si>
+    <t>Rite</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Asia Middle East</t>
+  </si>
+  <si>
+    <t>Asia South East Far East</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>PastCen A</t>
+  </si>
+  <si>
+    <t>PastCen avg per Dio</t>
+  </si>
+  <si>
+    <t>Inh per PastCen</t>
+  </si>
+  <si>
+    <t>Cath per PastCen</t>
+  </si>
+  <si>
+    <t>Parishes A</t>
+  </si>
+  <si>
+    <t>Parishes P</t>
+  </si>
+  <si>
+    <t>Mission Stations A</t>
+  </si>
+  <si>
+    <t>Mission Stations P</t>
+  </si>
+  <si>
+    <t>Other centres A</t>
+  </si>
+  <si>
+    <t>Other centres P</t>
+  </si>
+  <si>
+    <t>Tot A</t>
+  </si>
+  <si>
+    <t>Tot P</t>
+  </si>
+  <si>
+    <t>II-a</t>
+  </si>
+  <si>
+    <t>Bishops present on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Bp native tcor</t>
+  </si>
+  <si>
+    <t>Bpforeign tcor</t>
+  </si>
+  <si>
+    <t>Bp Tot</t>
+  </si>
+  <si>
+    <t>II-b</t>
+  </si>
+  <si>
+    <t>Number of priests (diocesan and religious) present - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of priests (diocesan and religious) present - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Index of pastoral workload - Catholics per priest (diocesan and religious)</t>
+  </si>
+  <si>
+    <t>Index of pastoral workload - Inhabitants per priest (diocesan and religious)</t>
+  </si>
+  <si>
+    <t>II-c</t>
+  </si>
+  <si>
+    <t>Number of diocesan priests present - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of diocesan priests present - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>II-d</t>
+  </si>
+  <si>
+    <t>Number of diocesan priests incardinated - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of diocesan priests incardinated - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>II-e</t>
+  </si>
+  <si>
+    <t>Number of religious priests present - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of religious priests present - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>II-f</t>
+  </si>
+  <si>
+    <t>Number of permanent deacons (diocesan and religious) - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of permanent deacons (diocesan and religious) - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>II-g</t>
+  </si>
+  <si>
+    <t>Number of lay men religious - absolute figures</t>
+  </si>
+  <si>
+    <t>II-h</t>
+  </si>
+  <si>
+    <t>Number of lay men religious - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Number of temporarily and perpetually professed women religious - absolute figures</t>
+  </si>
+  <si>
+    <t>II-i</t>
+  </si>
+  <si>
+    <t>II-l</t>
+  </si>
+  <si>
+    <t>II-m</t>
+  </si>
+  <si>
+    <t>Number of temporarily and perpetually professed women religious - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>Ordinations deaths an defections of diocesan priests as percentages of those incardinated at the beginning of 2022</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Ordinations deaths an defections of diocesan priests as percentages of those incardinated at the beginning of the year</t>
+  </si>
+  <si>
+    <t>III-a</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for philosophy and theology and for secondary-school students - diocesan and religious</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for philosophy and theology and for secondary-school students - diocesan</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for philosophy and theology and for secondary-school students - religious</t>
+  </si>
+  <si>
+    <t>III-b</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for philosophy and theology students (diocesan and religious) - seminaries and residences</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for philosophy and theology students (diocesan and religious) - seminaries</t>
+  </si>
+  <si>
+    <t>III-c</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for secondary-school students (diocesan and religious) - seminaries and residences</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for secondary-school students (diocesan and religious) - seminaries</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for secondary-school students (diocesan and religious) -residences</t>
+  </si>
+  <si>
+    <t>Diocesan training centres for priesthood, for philosophy and theology and for secondary-school students - seminaries</t>
+  </si>
+  <si>
+    <t>Diocesan training centres for priesthood, for philosophy and theology and for secondary-school students - residences</t>
+  </si>
+  <si>
+    <t>III-d</t>
+  </si>
+  <si>
+    <t>III-e</t>
+  </si>
+  <si>
+    <t>Religious training centres for priesthood, for philosophy and theology and for secondary-school students - seminaries</t>
+  </si>
+  <si>
+    <t>Religious training centres for priesthood, for philosophy and theology and for secondary-school students - residences</t>
+  </si>
+  <si>
+    <t>III-f</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in the philosophy and theology centres (diocesan and religious) - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in the philosophy and theology centres (diocesan and religious) - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>III-g</t>
+  </si>
+  <si>
+    <t>Training centres for priesthood, for philosophy and theology students (diocesan and religious) - residences</t>
+  </si>
+  <si>
+    <t>III-h</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in diocesan centres - philosophy and theology</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in the secondary-school centres (diocesan and religious) - absolute figures</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in diocesan centres - secondary schools</t>
+  </si>
+  <si>
+    <t>III-i</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in religious centres - secondary schools</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in religious centres - philosophy and theology</t>
+  </si>
+  <si>
+    <t>Number of candidates for priesthood in the secondary-school centres (diocesan and religious) - index numbers (base 2013 = 100)</t>
+  </si>
+  <si>
+    <t>III-l</t>
+  </si>
+  <si>
+    <t>Ordinations, deaths, and defections of diocesan priests as percentages of those incardinated at beginning of year 2022</t>
+  </si>
+  <si>
+    <t>Some significant data about papal-jurisdiction institutes for women - Autonomous Houses</t>
+  </si>
+  <si>
+    <t>Some significant data about papal-jurisdiction institutes for women - Centralized Institutes</t>
+  </si>
+  <si>
+    <t>Some significant data about papal-jurisdiction institutes for women - Secular Institutes</t>
+  </si>
+  <si>
+    <t>III-m</t>
+  </si>
+  <si>
+    <t>Ordination rate in diocesan centres (priestly ordinations per 100 philosophy and theology students)</t>
+  </si>
+  <si>
+    <t>III-n</t>
+  </si>
+  <si>
+    <t>Number of students in the diocesan philosophy and theology centres who left the seminary</t>
+  </si>
+  <si>
+    <t>III-o</t>
+  </si>
+  <si>
+    <t>III-p</t>
+  </si>
+  <si>
+    <t>Departure rate of students in the diocesan philosophy and theology centres (departures per 100 enrolled students)</t>
+  </si>
+  <si>
+    <t>Educational institutions, 31 December 2022</t>
+  </si>
+  <si>
+    <t>III-q</t>
+  </si>
+  <si>
+    <t>SecSc junior and senior Students</t>
+  </si>
+  <si>
+    <t>Percentage of people over seven years old among those receiving baptism</t>
+  </si>
+  <si>
+    <t>Percentage of marriages that are mixed marriages</t>
+  </si>
+  <si>
+    <t>IV-b</t>
+  </si>
+  <si>
+    <t>IV-a</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 - total</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 - depending on the Congregation for the Eastern Churches</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022 - depending on the Congregation for the Evangelization of Peoples</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of institutes, of houses, and of members on 31 December 2022  - depending on the Congregation for the Institutes of Consecrated and Societies of Apostolic life</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 - total</t>
+  </si>
+  <si>
+    <t>Number of novices in religious institutes for men - seminarians</t>
+  </si>
+  <si>
+    <t>Number of novices in religious institutes for men - others</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 - depending on the Congregation for the Eastern Churches</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 - depending on the Congregation for the Evangelization of Peoples</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for men. Number of novices on 31 December 2022 - depending on the Congregation for the Institutes of Consecrated and Societies of Apostolic life</t>
+  </si>
+  <si>
+    <t>COLUMNS…</t>
+  </si>
+  <si>
+    <t>Tables to be included: 27 (those split in several subtables are counted as one)</t>
+  </si>
+  <si>
+    <t>Tables to be included: 67 (if counting each subtable)</t>
+  </si>
+  <si>
+    <t>Tables to be included: 59 (if counting those split in several subtables as one)</t>
+  </si>
+  <si>
+    <t>Tables to be included: 39 (if counting each subtable)</t>
+  </si>
+  <si>
+    <t>Vocation rate (in the diocesan and religious centres) - number of philosophy and theology and secondary-school students per 100,000 Catholics</t>
+  </si>
+  <si>
+    <t>Vocation rate (in the diocesan and religious centres) - number of philosophy and theology and secondary-school students per 100,000 inhabitants</t>
+  </si>
+  <si>
+    <t>Vocation rate (in the diocesan and religious centres) - number of philosophy and theology students per 100,000 Catholics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1108,8 +1544,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,6 +1576,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1147,7 +1601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1164,11 +1618,28 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1503,40 +1974,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" customWidth="1"/>
     <col min="2" max="2" width="5.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>172</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="28" t="s">
         <v>164</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>281</v>
+      <c r="A3" s="21" t="s">
+        <v>314</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1573,8 +2044,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>282</v>
+      <c r="A4" s="21" t="s">
+        <v>315</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -1626,8 +2097,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>283</v>
+      <c r="A5" s="21" t="s">
+        <v>316</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
@@ -1661,8 +2132,8 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>284</v>
+      <c r="A6" s="21" t="s">
+        <v>253</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -1687,14 +2158,14 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="29" t="s">
         <v>165</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>285</v>
+      <c r="A8" s="22" t="s">
+        <v>317</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
@@ -1737,8 +2208,8 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>286</v>
+      <c r="A9" s="22" t="s">
+        <v>254</v>
       </c>
       <c r="B9" s="4">
         <v>6</v>
@@ -1757,8 +2228,8 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>287</v>
+      <c r="A10" s="22" t="s">
+        <v>318</v>
       </c>
       <c r="B10" s="4">
         <v>7</v>
@@ -1777,8 +2248,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>288</v>
+      <c r="A11" s="22" t="s">
+        <v>319</v>
       </c>
       <c r="B11" s="4">
         <v>8</v>
@@ -1818,8 +2289,8 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>289</v>
+      <c r="A12" s="22" t="s">
+        <v>320</v>
       </c>
       <c r="B12" s="4">
         <v>9</v>
@@ -1847,8 +2318,8 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>290</v>
+      <c r="A13" s="22" t="s">
+        <v>321</v>
       </c>
       <c r="B13" s="4">
         <v>10</v>
@@ -1873,8 +2344,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>291</v>
+      <c r="A14" s="22" t="s">
+        <v>255</v>
       </c>
       <c r="B14" s="4">
         <v>11</v>
@@ -1905,8 +2376,8 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>293</v>
+      <c r="A15" s="22" t="s">
+        <v>424</v>
       </c>
       <c r="B15" s="4">
         <v>12</v>
@@ -1928,7 +2399,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="22" t="s">
         <v>162</v>
       </c>
       <c r="B16" s="4">
@@ -1957,7 +2428,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="22" t="s">
         <v>163</v>
       </c>
       <c r="B17" s="4">
@@ -1986,8 +2457,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>173</v>
+      <c r="A18" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="B18" s="4">
         <v>15</v>
@@ -2015,8 +2486,8 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>174</v>
+      <c r="A19" s="22" t="s">
+        <v>173</v>
       </c>
       <c r="B19" s="4">
         <v>16</v>
@@ -2044,8 +2515,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>175</v>
+      <c r="A20" s="22" t="s">
+        <v>174</v>
       </c>
       <c r="B20" s="4">
         <v>17</v>
@@ -2073,8 +2544,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>176</v>
+      <c r="A21" s="22" t="s">
+        <v>175</v>
       </c>
       <c r="B21" s="4">
         <v>18</v>
@@ -2102,8 +2573,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>177</v>
+      <c r="A22" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="B22" s="4">
         <v>19</v>
@@ -2131,8 +2602,8 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>178</v>
+      <c r="A23" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="B23" s="4">
         <v>20</v>
@@ -2160,14 +2631,14 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="30" t="s">
         <v>166</v>
       </c>
       <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="B25" s="5">
         <v>21</v>
@@ -2202,7 +2673,7 @@
     </row>
     <row r="26" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>295</v>
+        <v>323</v>
       </c>
       <c r="B26" s="5">
         <v>22</v>
@@ -2249,7 +2720,7 @@
     </row>
     <row r="27" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>296</v>
+        <v>257</v>
       </c>
       <c r="B27" s="5">
         <v>23</v>
@@ -2269,7 +2740,7 @@
     </row>
     <row r="28" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>297</v>
+        <v>258</v>
       </c>
       <c r="B28" s="5">
         <v>24</v>
@@ -2289,7 +2760,7 @@
     </row>
     <row r="29" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="B29" s="5">
         <v>25</v>
@@ -2327,7 +2798,7 @@
     </row>
     <row r="30" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30" s="5">
         <v>26</v>
@@ -2356,7 +2827,7 @@
     </row>
     <row r="31" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B31" s="5">
         <v>27</v>
@@ -2385,7 +2856,7 @@
     </row>
     <row r="32" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B32" s="5">
         <v>28</v>
@@ -2414,7 +2885,7 @@
     </row>
     <row r="33" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" s="5">
         <v>29</v>
@@ -2442,14 +2913,14 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="32" t="s">
         <v>167</v>
       </c>
       <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19" t="s">
-        <v>299</v>
+      <c r="A35" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="B35" s="6">
         <v>30</v>
@@ -2483,8 +2954,8 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19" t="s">
-        <v>300</v>
+      <c r="A36" s="17" t="s">
+        <v>260</v>
       </c>
       <c r="B36" s="6">
         <v>31</v>
@@ -2506,8 +2977,8 @@
       </c>
     </row>
     <row r="37" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
-        <v>301</v>
+      <c r="A37" s="17" t="s">
+        <v>261</v>
       </c>
       <c r="B37" s="6">
         <v>32</v>
@@ -2553,14 +3024,14 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="31" t="s">
         <v>168</v>
       </c>
       <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
-        <v>302</v>
+      <c r="A39" s="18" t="s">
+        <v>325</v>
       </c>
       <c r="B39" s="7">
         <v>33</v>
@@ -2580,7 +3051,7 @@
       <c r="G39" t="s">
         <v>147</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" t="s">
         <v>148</v>
       </c>
       <c r="I39" t="s">
@@ -2606,8 +3077,8 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>183</v>
+      <c r="A41" s="27" t="s">
+        <v>442</v>
       </c>
       <c r="B41" s="8">
         <v>34</v>
@@ -2641,8 +3112,8 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
-        <v>184</v>
+      <c r="A42" s="27" t="s">
+        <v>443</v>
       </c>
       <c r="B42" s="8">
         <v>34</v>
@@ -2676,8 +3147,8 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
-        <v>185</v>
+      <c r="A43" s="27" t="s">
+        <v>444</v>
       </c>
       <c r="B43" s="8">
         <v>34</v>
@@ -2711,8 +3182,8 @@
       </c>
     </row>
     <row r="44" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
-        <v>186</v>
+      <c r="A44" s="27" t="s">
+        <v>445</v>
       </c>
       <c r="B44" s="8">
         <v>34</v>
@@ -2746,8 +3217,8 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
-        <v>190</v>
+      <c r="A45" s="27" t="s">
+        <v>446</v>
       </c>
       <c r="B45" s="8">
         <v>35</v>
@@ -2756,18 +3227,18 @@
         <v>153</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E45" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F45" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
-        <v>191</v>
+      <c r="A46" s="27" t="s">
+        <v>449</v>
       </c>
       <c r="B46" s="8">
         <v>35</v>
@@ -2776,18 +3247,18 @@
         <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E46" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F46" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13" t="s">
-        <v>219</v>
+      <c r="A47" s="27" t="s">
+        <v>450</v>
       </c>
       <c r="B47" s="8">
         <v>35</v>
@@ -2796,18 +3267,18 @@
         <v>153</v>
       </c>
       <c r="D47" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E47" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F47" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>220</v>
+      <c r="A48" s="27" t="s">
+        <v>451</v>
       </c>
       <c r="B48" s="8">
         <v>35</v>
@@ -2816,18 +3287,18 @@
         <v>153</v>
       </c>
       <c r="D48" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E48" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F48" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>303</v>
+      <c r="A49" s="27" t="s">
+        <v>326</v>
       </c>
       <c r="B49" s="8">
         <v>36</v>
@@ -2842,30 +3313,30 @@
         <v>37</v>
       </c>
       <c r="F49" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="G49" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="H49" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="I49" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="J49" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K49" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="L49" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>207</v>
+      <c r="A50" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="B50" s="8">
         <v>37</v>
@@ -2877,27 +3348,27 @@
         <v>74</v>
       </c>
       <c r="E50" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F50" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G50" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="H50" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="I50" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J50" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
-        <v>208</v>
+      <c r="A51" s="27" t="s">
+        <v>201</v>
       </c>
       <c r="B51" s="8">
         <v>39</v>
@@ -2906,33 +3377,33 @@
         <v>153</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F51" t="s">
+        <v>190</v>
+      </c>
+      <c r="G51" t="s">
         <v>197</v>
       </c>
-      <c r="G51" t="s">
-        <v>204</v>
-      </c>
       <c r="H51" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I51" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J51" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K51" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
-        <v>304</v>
+      <c r="A52" s="27" t="s">
+        <v>327</v>
       </c>
       <c r="B52" s="8">
         <v>40</v>
@@ -2944,21 +3415,21 @@
         <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F52" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="G52" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H52" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>305</v>
+      <c r="A53" s="27" t="s">
+        <v>328</v>
       </c>
       <c r="B53" s="8">
         <v>41</v>
@@ -2967,21 +3438,21 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E53" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F53" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="G53" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>216</v>
+      <c r="A54" s="27" t="s">
+        <v>297</v>
       </c>
       <c r="B54" s="8">
         <v>42</v>
@@ -3010,7 +3481,7 @@
     </row>
     <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>217</v>
+        <v>298</v>
       </c>
       <c r="B55" s="8">
         <v>42</v>
@@ -3038,8 +3509,8 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>218</v>
+      <c r="A56" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="B56" s="8">
         <v>43</v>
@@ -3068,7 +3539,7 @@
     </row>
     <row r="57" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>222</v>
+        <v>299</v>
       </c>
       <c r="B57" s="8">
         <v>43</v>
@@ -3096,8 +3567,8 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>223</v>
+      <c r="A58" s="27" t="s">
+        <v>306</v>
       </c>
       <c r="B58" s="8">
         <v>44</v>
@@ -3126,7 +3597,7 @@
     </row>
     <row r="59" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>224</v>
+        <v>300</v>
       </c>
       <c r="B59" s="8">
         <v>44</v>
@@ -3154,8 +3625,8 @@
       </c>
     </row>
     <row r="60" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
-        <v>225</v>
+      <c r="A60" s="27" t="s">
+        <v>307</v>
       </c>
       <c r="B60" s="8">
         <v>45</v>
@@ -3184,7 +3655,7 @@
     </row>
     <row r="61" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>226</v>
+        <v>301</v>
       </c>
       <c r="B61" s="8">
         <v>45</v>
@@ -3212,8 +3683,8 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
-        <v>227</v>
+      <c r="A62" s="27" t="s">
+        <v>310</v>
       </c>
       <c r="B62" s="8">
         <v>46</v>
@@ -3242,7 +3713,7 @@
     </row>
     <row r="63" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="B63" s="8">
         <v>46</v>
@@ -3270,8 +3741,8 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
-        <v>229</v>
+      <c r="A64" s="27" t="s">
+        <v>309</v>
       </c>
       <c r="B64" s="8">
         <v>47</v>
@@ -3300,7 +3771,7 @@
     </row>
     <row r="65" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="B65" s="8">
         <v>47</v>
@@ -3328,8 +3799,8 @@
       </c>
     </row>
     <row r="66" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
-        <v>231</v>
+      <c r="A66" s="27" t="s">
+        <v>308</v>
       </c>
       <c r="B66" s="8">
         <v>48</v>
@@ -3358,7 +3829,7 @@
     </row>
     <row r="67" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>232</v>
+        <v>304</v>
       </c>
       <c r="B67" s="8">
         <v>48</v>
@@ -3386,8 +3857,8 @@
       </c>
     </row>
     <row r="68" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="13" t="s">
-        <v>233</v>
+      <c r="A68" s="27" t="s">
+        <v>447</v>
       </c>
       <c r="B68" s="8">
         <v>49</v>
@@ -3415,8 +3886,8 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13" t="s">
-        <v>234</v>
+      <c r="A69" s="27" t="s">
+        <v>448</v>
       </c>
       <c r="B69" s="8">
         <v>49</v>
@@ -3444,14 +3915,14 @@
       </c>
     </row>
     <row r="70" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="13" t="s">
-        <v>235</v>
+      <c r="A70" s="27" t="s">
+        <v>425</v>
       </c>
       <c r="B70" s="8">
         <v>50</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D70">
         <v>2017</v>
@@ -3473,14 +3944,14 @@
       </c>
     </row>
     <row r="71" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="13" t="s">
-        <v>236</v>
+      <c r="A71" s="27" t="s">
+        <v>426</v>
       </c>
       <c r="B71" s="8">
         <v>50</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="D71">
         <v>2017</v>
@@ -3502,14 +3973,14 @@
       </c>
     </row>
     <row r="72" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="13" t="s">
-        <v>237</v>
+      <c r="A72" s="27" t="s">
+        <v>427</v>
       </c>
       <c r="B72" s="8">
         <v>50</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="D72">
         <v>2017</v>
@@ -3531,13 +4002,13 @@
       </c>
     </row>
     <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="14" t="s">
-        <v>238</v>
+      <c r="A73" s="33" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
       <c r="B74" s="14">
         <v>51</v>
@@ -3546,33 +4017,33 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="E74" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="F74" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="G74" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="H74" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="I74" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="J74" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="K74" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
-        <v>307</v>
+        <v>263</v>
       </c>
       <c r="B75" s="14">
         <v>52</v>
@@ -3581,33 +4052,33 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="E75" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="F75" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="G75" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="H75" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="I75" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="J75" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="K75" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
-        <v>308</v>
+        <v>264</v>
       </c>
       <c r="B76" s="14">
         <v>53</v>
@@ -3616,33 +4087,33 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="E76" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="F76" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="G76" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="H76" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="I76" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="J76" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="K76" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="B77" s="14">
         <v>54</v>
@@ -3651,42 +4122,42 @@
         <v>0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="E77" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="F77" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="G77" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="H77" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="I77" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="J77" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="K77" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="L77" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="M77" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="N77" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="B78" s="14">
         <v>55</v>
@@ -3695,39 +4166,39 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="E78" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="F78" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="G78" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="H78" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="I78" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="J78" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="K78" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="L78" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="M78" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
-        <v>311</v>
+        <v>267</v>
       </c>
       <c r="B79" s="14">
         <v>56</v>
@@ -3736,39 +4207,39 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="E79" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="F79" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="G79" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="H79" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="I79" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="J79" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="K79" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="L79" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="M79" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
-        <v>312</v>
+        <v>268</v>
       </c>
       <c r="B80" s="14">
         <v>57</v>
@@ -3777,27 +4248,27 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="E80" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="F80" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="G80" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="H80" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="I80" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
-        <v>313</v>
+        <v>269</v>
       </c>
       <c r="B81" s="14">
         <v>58</v>
@@ -3806,21 +4277,21 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="E81" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="F81" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="G81" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="s">
-        <v>314</v>
+        <v>270</v>
       </c>
       <c r="B82" s="14">
         <v>59</v>
@@ -3829,32 +4300,2097 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
+        <v>244</v>
+      </c>
+      <c r="E82" t="s">
+        <v>245</v>
+      </c>
+      <c r="F82" t="s">
+        <v>246</v>
+      </c>
+      <c r="G82" t="s">
+        <v>247</v>
+      </c>
+      <c r="H82" t="s">
+        <v>248</v>
+      </c>
+      <c r="I82" t="s">
+        <v>249</v>
+      </c>
+      <c r="J82" t="s">
+        <v>250</v>
+      </c>
+      <c r="K82" t="s">
+        <v>251</v>
+      </c>
+      <c r="L82" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="34" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="34" t="s">
+        <v>454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
+  <dimension ref="A1:K85"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="E82" t="s">
+      <c r="B3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="F82" t="s">
+      <c r="C4" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" t="s">
+        <v>337</v>
+      </c>
+      <c r="E4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F4" t="s">
+        <v>339</v>
+      </c>
+      <c r="G4" t="s">
+        <v>340</v>
+      </c>
+      <c r="H4" t="s">
+        <v>341</v>
+      </c>
+      <c r="I4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E5" t="s">
+        <v>338</v>
+      </c>
+      <c r="F5" t="s">
+        <v>339</v>
+      </c>
+      <c r="G5" t="s">
+        <v>340</v>
+      </c>
+      <c r="H5" t="s">
+        <v>341</v>
+      </c>
+      <c r="I5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="G82" t="s">
+      <c r="C6" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6">
+        <v>2017</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+      <c r="F6">
+        <v>2019</v>
+      </c>
+      <c r="G6">
+        <v>2020</v>
+      </c>
+      <c r="H6">
+        <v>2021</v>
+      </c>
+      <c r="I6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7">
+        <v>2017</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+      <c r="F7">
+        <v>2019</v>
+      </c>
+      <c r="G7">
+        <v>2020</v>
+      </c>
+      <c r="H7">
+        <v>2021</v>
+      </c>
+      <c r="I7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="H82" t="s">
-        <v>276</v>
-      </c>
-      <c r="I82" t="s">
+      <c r="C8" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8">
+        <v>2017</v>
+      </c>
+      <c r="E8">
+        <v>2018</v>
+      </c>
+      <c r="F8">
+        <v>2019</v>
+      </c>
+      <c r="G8">
+        <v>2020</v>
+      </c>
+      <c r="H8">
+        <v>2021</v>
+      </c>
+      <c r="I8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="J82" t="s">
+      <c r="C9" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="D9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E9" t="s">
+        <v>345</v>
+      </c>
+      <c r="F9" t="s">
+        <v>346</v>
+      </c>
+      <c r="G9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="K82" t="s">
+      <c r="B10" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="L82" t="s">
+      <c r="C10" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D10" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" t="s">
+        <v>349</v>
+      </c>
+      <c r="G10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>280</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11">
+        <v>2017</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>2019</v>
+      </c>
+      <c r="G11">
+        <v>2020</v>
+      </c>
+      <c r="H11">
+        <v>2021</v>
+      </c>
+      <c r="I11">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" t="s">
+        <v>351</v>
+      </c>
+      <c r="E12" t="s">
+        <v>352</v>
+      </c>
+      <c r="F12" t="s">
+        <v>353</v>
+      </c>
+      <c r="G12" t="s">
+        <v>354</v>
+      </c>
+      <c r="H12" t="s">
+        <v>355</v>
+      </c>
+      <c r="I12" t="s">
+        <v>356</v>
+      </c>
+      <c r="J12" t="s">
+        <v>357</v>
+      </c>
+      <c r="K12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D13">
+        <v>2017</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
+        <v>2019</v>
+      </c>
+      <c r="G13">
+        <v>2020</v>
+      </c>
+      <c r="H13">
+        <v>2021</v>
+      </c>
+      <c r="I13">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14">
+        <v>2017</v>
+      </c>
+      <c r="E14">
+        <v>2018</v>
+      </c>
+      <c r="F14">
+        <v>2019</v>
+      </c>
+      <c r="G14">
+        <v>2020</v>
+      </c>
+      <c r="H14">
+        <v>2021</v>
+      </c>
+      <c r="I14">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15">
+        <v>2017</v>
+      </c>
+      <c r="E15">
+        <v>2018</v>
+      </c>
+      <c r="F15">
+        <v>2019</v>
+      </c>
+      <c r="G15">
+        <v>2020</v>
+      </c>
+      <c r="H15">
+        <v>2021</v>
+      </c>
+      <c r="I15">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16">
+        <v>2017</v>
+      </c>
+      <c r="E16">
+        <v>2018</v>
+      </c>
+      <c r="F16">
+        <v>2019</v>
+      </c>
+      <c r="G16">
+        <v>2020</v>
+      </c>
+      <c r="H16">
+        <v>2021</v>
+      </c>
+      <c r="I16">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17">
+        <v>2017</v>
+      </c>
+      <c r="E17">
+        <v>2017</v>
+      </c>
+      <c r="F17">
+        <v>2019</v>
+      </c>
+      <c r="G17">
+        <v>2020</v>
+      </c>
+      <c r="H17">
+        <v>2021</v>
+      </c>
+      <c r="I17">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D18">
+        <v>2017</v>
+      </c>
+      <c r="E18">
+        <v>2018</v>
+      </c>
+      <c r="F18">
+        <v>2019</v>
+      </c>
+      <c r="G18">
+        <v>2020</v>
+      </c>
+      <c r="H18">
+        <v>2021</v>
+      </c>
+      <c r="I18">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D19">
+        <v>2017</v>
+      </c>
+      <c r="E19">
+        <v>2018</v>
+      </c>
+      <c r="F19">
+        <v>2019</v>
+      </c>
+      <c r="G19">
+        <v>2020</v>
+      </c>
+      <c r="H19">
+        <v>2021</v>
+      </c>
+      <c r="I19">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D20">
+        <v>2017</v>
+      </c>
+      <c r="E20">
+        <v>2018</v>
+      </c>
+      <c r="F20">
+        <v>2019</v>
+      </c>
+      <c r="G20">
+        <v>2020</v>
+      </c>
+      <c r="H20">
+        <v>2021</v>
+      </c>
+      <c r="I20">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D22" t="s">
+        <v>361</v>
+      </c>
+      <c r="E22" t="s">
+        <v>362</v>
+      </c>
+      <c r="F22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D23">
+        <v>2017</v>
+      </c>
+      <c r="E23">
+        <v>2018</v>
+      </c>
+      <c r="F23">
+        <v>2019</v>
+      </c>
+      <c r="G23">
+        <v>2020</v>
+      </c>
+      <c r="H23">
+        <v>2021</v>
+      </c>
+      <c r="I23">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D24">
+        <v>2017</v>
+      </c>
+      <c r="E24">
+        <v>2018</v>
+      </c>
+      <c r="F24">
+        <v>2019</v>
+      </c>
+      <c r="G24">
+        <v>2020</v>
+      </c>
+      <c r="H24">
+        <v>2021</v>
+      </c>
+      <c r="I24">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D25">
+        <v>2017</v>
+      </c>
+      <c r="E25">
+        <v>2018</v>
+      </c>
+      <c r="F25">
+        <v>2019</v>
+      </c>
+      <c r="G25">
+        <v>2020</v>
+      </c>
+      <c r="H25">
+        <v>2021</v>
+      </c>
+      <c r="I25">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D26">
+        <v>2017</v>
+      </c>
+      <c r="E26">
+        <v>2018</v>
+      </c>
+      <c r="F26">
+        <v>2019</v>
+      </c>
+      <c r="G26">
+        <v>2020</v>
+      </c>
+      <c r="H26">
+        <v>2021</v>
+      </c>
+      <c r="I26">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D27">
+        <v>2017</v>
+      </c>
+      <c r="E27">
+        <v>2018</v>
+      </c>
+      <c r="F27">
+        <v>2019</v>
+      </c>
+      <c r="G27">
+        <v>2020</v>
+      </c>
+      <c r="H27">
+        <v>2021</v>
+      </c>
+      <c r="I27">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D28">
+        <v>2017</v>
+      </c>
+      <c r="E28">
+        <v>2018</v>
+      </c>
+      <c r="F28">
+        <v>2019</v>
+      </c>
+      <c r="G28">
+        <v>2020</v>
+      </c>
+      <c r="H28">
+        <v>2021</v>
+      </c>
+      <c r="I28">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29">
+        <v>2017</v>
+      </c>
+      <c r="E29">
+        <v>2018</v>
+      </c>
+      <c r="F29">
+        <v>2019</v>
+      </c>
+      <c r="G29">
+        <v>2020</v>
+      </c>
+      <c r="H29">
+        <v>2021</v>
+      </c>
+      <c r="I29">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D30">
+        <v>2017</v>
+      </c>
+      <c r="E30">
+        <v>2018</v>
+      </c>
+      <c r="F30">
+        <v>2019</v>
+      </c>
+      <c r="G30">
+        <v>2020</v>
+      </c>
+      <c r="H30">
+        <v>2021</v>
+      </c>
+      <c r="I30">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31">
+        <v>2017</v>
+      </c>
+      <c r="E31">
+        <v>2018</v>
+      </c>
+      <c r="F31">
+        <v>2019</v>
+      </c>
+      <c r="G31">
+        <v>2020</v>
+      </c>
+      <c r="H31">
+        <v>2021</v>
+      </c>
+      <c r="I31">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D32">
+        <v>2017</v>
+      </c>
+      <c r="E32">
+        <v>2018</v>
+      </c>
+      <c r="F32">
+        <v>2019</v>
+      </c>
+      <c r="G32">
+        <v>2020</v>
+      </c>
+      <c r="H32">
+        <v>2021</v>
+      </c>
+      <c r="I32">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D33">
+        <v>2017</v>
+      </c>
+      <c r="E33">
+        <v>2018</v>
+      </c>
+      <c r="F33">
+        <v>2019</v>
+      </c>
+      <c r="G33">
+        <v>2020</v>
+      </c>
+      <c r="H33">
+        <v>2021</v>
+      </c>
+      <c r="I33">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D34">
+        <v>2017</v>
+      </c>
+      <c r="E34">
+        <v>2018</v>
+      </c>
+      <c r="F34">
+        <v>2019</v>
+      </c>
+      <c r="G34">
+        <v>2020</v>
+      </c>
+      <c r="H34">
+        <v>2021</v>
+      </c>
+      <c r="I34">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D35">
+        <v>2017</v>
+      </c>
+      <c r="E35">
+        <v>2018</v>
+      </c>
+      <c r="F35">
+        <v>2019</v>
+      </c>
+      <c r="G35">
+        <v>2020</v>
+      </c>
+      <c r="H35">
+        <v>2021</v>
+      </c>
+      <c r="I35">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D36">
+        <v>2017</v>
+      </c>
+      <c r="E36">
+        <v>2018</v>
+      </c>
+      <c r="F36">
+        <v>2019</v>
+      </c>
+      <c r="G36">
+        <v>2020</v>
+      </c>
+      <c r="H36">
+        <v>2021</v>
+      </c>
+      <c r="I36">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D37">
+        <v>2017</v>
+      </c>
+      <c r="E37">
+        <v>2018</v>
+      </c>
+      <c r="F37">
+        <v>2019</v>
+      </c>
+      <c r="G37">
+        <v>2020</v>
+      </c>
+      <c r="H37">
+        <v>2021</v>
+      </c>
+      <c r="I37">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D38">
+        <v>2017</v>
+      </c>
+      <c r="E38">
+        <v>2018</v>
+      </c>
+      <c r="F38">
+        <v>2019</v>
+      </c>
+      <c r="G38">
+        <v>2020</v>
+      </c>
+      <c r="H38">
+        <v>2021</v>
+      </c>
+      <c r="I38">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="D40" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D42">
+        <v>2017</v>
+      </c>
+      <c r="E42">
+        <v>2018</v>
+      </c>
+      <c r="F42">
+        <v>2019</v>
+      </c>
+      <c r="G42">
+        <v>2020</v>
+      </c>
+      <c r="H42">
+        <v>2021</v>
+      </c>
+      <c r="I42">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D43">
+        <v>2017</v>
+      </c>
+      <c r="E43">
+        <v>2018</v>
+      </c>
+      <c r="F43">
+        <v>2019</v>
+      </c>
+      <c r="G43">
+        <v>2020</v>
+      </c>
+      <c r="H43">
+        <v>2021</v>
+      </c>
+      <c r="I43">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D44">
+        <v>2017</v>
+      </c>
+      <c r="E44">
+        <v>2018</v>
+      </c>
+      <c r="F44">
+        <v>2019</v>
+      </c>
+      <c r="G44">
+        <v>2020</v>
+      </c>
+      <c r="H44">
+        <v>2021</v>
+      </c>
+      <c r="I44">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D45">
+        <v>2017</v>
+      </c>
+      <c r="E45">
+        <v>2018</v>
+      </c>
+      <c r="F45">
+        <v>2019</v>
+      </c>
+      <c r="G45">
+        <v>2020</v>
+      </c>
+      <c r="H45">
+        <v>2021</v>
+      </c>
+      <c r="I45">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D46">
+        <v>2017</v>
+      </c>
+      <c r="E46">
+        <v>2018</v>
+      </c>
+      <c r="F46">
+        <v>2019</v>
+      </c>
+      <c r="G46">
+        <v>2020</v>
+      </c>
+      <c r="H46">
+        <v>2021</v>
+      </c>
+      <c r="I46">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D47">
+        <v>2017</v>
+      </c>
+      <c r="E47">
+        <v>2018</v>
+      </c>
+      <c r="F47">
+        <v>2019</v>
+      </c>
+      <c r="G47" s="20">
+        <v>2020</v>
+      </c>
+      <c r="H47">
+        <v>2021</v>
+      </c>
+      <c r="I47">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D48">
+        <v>2017</v>
+      </c>
+      <c r="E48">
+        <v>2018</v>
+      </c>
+      <c r="F48">
+        <v>2019</v>
+      </c>
+      <c r="G48">
+        <v>2020</v>
+      </c>
+      <c r="H48">
+        <v>2021</v>
+      </c>
+      <c r="I48">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D49">
+        <v>2017</v>
+      </c>
+      <c r="E49">
+        <v>2018</v>
+      </c>
+      <c r="F49">
+        <v>2019</v>
+      </c>
+      <c r="G49">
+        <v>2020</v>
+      </c>
+      <c r="H49">
+        <v>2021</v>
+      </c>
+      <c r="I49">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D50">
+        <v>2017</v>
+      </c>
+      <c r="E50">
+        <v>2018</v>
+      </c>
+      <c r="F50">
+        <v>2019</v>
+      </c>
+      <c r="G50">
+        <v>2020</v>
+      </c>
+      <c r="H50">
+        <v>2021</v>
+      </c>
+      <c r="I50">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D51">
+        <v>2017</v>
+      </c>
+      <c r="E51">
+        <v>2018</v>
+      </c>
+      <c r="F51">
+        <v>2019</v>
+      </c>
+      <c r="G51">
+        <v>2020</v>
+      </c>
+      <c r="H51">
+        <v>2021</v>
+      </c>
+      <c r="I51">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D52">
+        <v>2017</v>
+      </c>
+      <c r="E52">
+        <v>2018</v>
+      </c>
+      <c r="F52">
+        <v>2019</v>
+      </c>
+      <c r="G52">
+        <v>2020</v>
+      </c>
+      <c r="H52">
+        <v>2021</v>
+      </c>
+      <c r="I52">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D53">
+        <v>2017</v>
+      </c>
+      <c r="E53">
+        <v>2018</v>
+      </c>
+      <c r="F53">
+        <v>2019</v>
+      </c>
+      <c r="G53">
+        <v>2020</v>
+      </c>
+      <c r="H53">
+        <v>2021</v>
+      </c>
+      <c r="I53">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D54">
+        <v>2017</v>
+      </c>
+      <c r="E54">
+        <v>2018</v>
+      </c>
+      <c r="F54">
+        <v>2019</v>
+      </c>
+      <c r="G54">
+        <v>2020</v>
+      </c>
+      <c r="H54">
+        <v>2021</v>
+      </c>
+      <c r="I54">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="35" t="s">
+        <v>411</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D55">
+        <v>2017</v>
+      </c>
+      <c r="E55">
+        <v>2018</v>
+      </c>
+      <c r="F55">
+        <v>2019</v>
+      </c>
+      <c r="G55">
+        <v>2020</v>
+      </c>
+      <c r="H55">
+        <v>2021</v>
+      </c>
+      <c r="I55">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D56">
+        <v>2017</v>
+      </c>
+      <c r="E56">
+        <v>2018</v>
+      </c>
+      <c r="F56">
+        <v>2019</v>
+      </c>
+      <c r="G56">
+        <v>2020</v>
+      </c>
+      <c r="H56">
+        <v>2021</v>
+      </c>
+      <c r="I56">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="35" t="s">
+        <v>417</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D57">
+        <v>2017</v>
+      </c>
+      <c r="E57">
+        <v>2018</v>
+      </c>
+      <c r="F57">
+        <v>2019</v>
+      </c>
+      <c r="G57">
+        <v>2020</v>
+      </c>
+      <c r="H57">
+        <v>2021</v>
+      </c>
+      <c r="I57">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D58">
+        <v>2017</v>
+      </c>
+      <c r="E58">
+        <v>2018</v>
+      </c>
+      <c r="F58">
+        <v>2019</v>
+      </c>
+      <c r="G58">
+        <v>2020</v>
+      </c>
+      <c r="H58">
+        <v>2021</v>
+      </c>
+      <c r="I58">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D59">
+        <v>2017</v>
+      </c>
+      <c r="E59">
+        <v>2018</v>
+      </c>
+      <c r="F59">
+        <v>2019</v>
+      </c>
+      <c r="G59">
+        <v>2020</v>
+      </c>
+      <c r="H59">
+        <v>2021</v>
+      </c>
+      <c r="I59">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D60">
+        <v>2017</v>
+      </c>
+      <c r="E60">
+        <v>2018</v>
+      </c>
+      <c r="F60">
+        <v>2019</v>
+      </c>
+      <c r="G60">
+        <v>2020</v>
+      </c>
+      <c r="H60">
+        <v>2021</v>
+      </c>
+      <c r="I60">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D61">
+        <v>2017</v>
+      </c>
+      <c r="E61">
+        <v>2018</v>
+      </c>
+      <c r="F61">
+        <v>2019</v>
+      </c>
+      <c r="G61">
+        <v>2020</v>
+      </c>
+      <c r="H61">
+        <v>2021</v>
+      </c>
+      <c r="I61">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D62">
+        <v>2017</v>
+      </c>
+      <c r="E62">
+        <v>2018</v>
+      </c>
+      <c r="F62">
+        <v>2019</v>
+      </c>
+      <c r="G62">
+        <v>2020</v>
+      </c>
+      <c r="H62">
+        <v>2021</v>
+      </c>
+      <c r="I62">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="25" t="s">
+        <v>457</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D63">
+        <v>2017</v>
+      </c>
+      <c r="E63">
+        <v>2018</v>
+      </c>
+      <c r="F63">
+        <v>2019</v>
+      </c>
+      <c r="G63">
+        <v>2020</v>
+      </c>
+      <c r="H63">
+        <v>2021</v>
+      </c>
+      <c r="I63">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D64">
+        <v>2017</v>
+      </c>
+      <c r="E64">
+        <v>2018</v>
+      </c>
+      <c r="F64">
+        <v>2019</v>
+      </c>
+      <c r="G64">
+        <v>2020</v>
+      </c>
+      <c r="H64">
+        <v>2021</v>
+      </c>
+      <c r="I64">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D65">
+        <v>2017</v>
+      </c>
+      <c r="E65">
+        <v>2018</v>
+      </c>
+      <c r="F65">
+        <v>2019</v>
+      </c>
+      <c r="G65">
+        <v>2020</v>
+      </c>
+      <c r="H65">
+        <v>2021</v>
+      </c>
+      <c r="I65">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D66">
+        <v>2017</v>
+      </c>
+      <c r="E66">
+        <v>2018</v>
+      </c>
+      <c r="F66">
+        <v>2019</v>
+      </c>
+      <c r="G66">
+        <v>2020</v>
+      </c>
+      <c r="H66">
+        <v>2021</v>
+      </c>
+      <c r="I66">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D67">
+        <v>2017</v>
+      </c>
+      <c r="E67">
+        <v>2018</v>
+      </c>
+      <c r="F67">
+        <v>2019</v>
+      </c>
+      <c r="G67">
+        <v>2020</v>
+      </c>
+      <c r="H67">
+        <v>2021</v>
+      </c>
+      <c r="I67">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D68">
+        <v>2017</v>
+      </c>
+      <c r="E68">
+        <v>2018</v>
+      </c>
+      <c r="F68">
+        <v>2019</v>
+      </c>
+      <c r="G68">
+        <v>2020</v>
+      </c>
+      <c r="H68">
+        <v>2021</v>
+      </c>
+      <c r="I68">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D69">
+        <v>2017</v>
+      </c>
+      <c r="E69">
+        <v>2018</v>
+      </c>
+      <c r="F69">
+        <v>2019</v>
+      </c>
+      <c r="G69">
+        <v>2020</v>
+      </c>
+      <c r="H69">
+        <v>2021</v>
+      </c>
+      <c r="I69">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D70" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70" t="s">
+        <v>114</v>
+      </c>
+      <c r="H70" t="s">
+        <v>115</v>
+      </c>
+      <c r="I70" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="37" t="s">
+        <v>438</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D72">
+        <v>2017</v>
+      </c>
+      <c r="E72">
+        <v>2018</v>
+      </c>
+      <c r="F72">
+        <v>2019</v>
+      </c>
+      <c r="G72">
+        <v>2020</v>
+      </c>
+      <c r="H72">
+        <v>2021</v>
+      </c>
+      <c r="I72">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="37" t="s">
+        <v>439</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73">
+        <v>2017</v>
+      </c>
+      <c r="E73">
+        <v>2018</v>
+      </c>
+      <c r="F73">
+        <v>2019</v>
+      </c>
+      <c r="G73">
+        <v>2020</v>
+      </c>
+      <c r="H73">
+        <v>2021</v>
+      </c>
+      <c r="I73">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="6"/>
+    </row>
+    <row r="75" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" s="7"/>
+    </row>
+    <row r="76" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="15"/>
+      <c r="B77" s="14"/>
+    </row>
+    <row r="78" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="B78" s="14"/>
+    </row>
+    <row r="79" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="B79" s="14"/>
+    </row>
+    <row r="80" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="15"/>
+      <c r="B80" s="14"/>
+      <c r="D80" s="20"/>
+    </row>
+    <row r="81" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="15"/>
+      <c r="B81" s="14"/>
+    </row>
+    <row r="82" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="15"/>
+      <c r="B82" s="14"/>
+    </row>
+    <row r="83" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="15"/>
+      <c r="B83" s="14"/>
+    </row>
+    <row r="84" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="15"/>
+      <c r="B84" s="14"/>
+    </row>
+    <row r="85" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="15"/>
+      <c r="B85" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrected data overview.xlsx (table was missing)
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D9AF8F-182A-429F-A848-46F113D19991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FDCEF-EE72-40F4-91CC-7749EA490AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="462">
   <si>
     <t>Countries</t>
   </si>
@@ -1401,9 +1401,6 @@
     <t>Tables to be included: 27 (those split in several subtables are counted as one)</t>
   </si>
   <si>
-    <t>Tables to be included: 67 (if counting each subtable)</t>
-  </si>
-  <si>
     <t>Tables to be included: 59 (if counting those split in several subtables as one)</t>
   </si>
   <si>
@@ -1417,6 +1414,15 @@
   </si>
   <si>
     <t>Vocation rate (in the diocesan and religious centres) - number of philosophy and theology students per 100,000 Catholics</t>
+  </si>
+  <si>
+    <t>Prefessed Relig Perp Vow</t>
+  </si>
+  <si>
+    <t>Papal-jurisdiction institutes for women: autonomous houses. Number of houses, novices, and professed religious on 31 December 2022</t>
+  </si>
+  <si>
+    <t>Tables to be included: 68 (if counting each subtable)</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1621,14 +1627,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1638,8 +1639,7 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1974,9 +1974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2000,13 +2002,13 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="23" t="s">
         <v>164</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="16" t="s">
         <v>314</v>
       </c>
       <c r="B3" s="3">
@@ -2044,7 +2046,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="16" t="s">
         <v>315</v>
       </c>
       <c r="B4" s="3">
@@ -2097,7 +2099,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="16" t="s">
         <v>316</v>
       </c>
       <c r="B5" s="3">
@@ -2132,7 +2134,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="16" t="s">
         <v>253</v>
       </c>
       <c r="B6" s="3">
@@ -2158,13 +2160,13 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="24" t="s">
         <v>165</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="11" t="s">
         <v>317</v>
       </c>
       <c r="B8" s="4">
@@ -2208,7 +2210,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="11" t="s">
         <v>254</v>
       </c>
       <c r="B9" s="4">
@@ -2228,7 +2230,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="11" t="s">
         <v>318</v>
       </c>
       <c r="B10" s="4">
@@ -2248,7 +2250,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="11" t="s">
         <v>319</v>
       </c>
       <c r="B11" s="4">
@@ -2289,7 +2291,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="11" t="s">
         <v>320</v>
       </c>
       <c r="B12" s="4">
@@ -2318,7 +2320,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="11" t="s">
         <v>321</v>
       </c>
       <c r="B13" s="4">
@@ -2344,7 +2346,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="11" t="s">
         <v>255</v>
       </c>
       <c r="B14" s="4">
@@ -2376,7 +2378,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="11" t="s">
         <v>424</v>
       </c>
       <c r="B15" s="4">
@@ -2399,7 +2401,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B16" s="4">
@@ -2428,7 +2430,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="11" t="s">
         <v>163</v>
       </c>
       <c r="B17" s="4">
@@ -2457,7 +2459,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="11" t="s">
         <v>172</v>
       </c>
       <c r="B18" s="4">
@@ -2486,7 +2488,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="11" t="s">
         <v>173</v>
       </c>
       <c r="B19" s="4">
@@ -2515,7 +2517,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B20" s="4">
@@ -2544,7 +2546,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="11" t="s">
         <v>175</v>
       </c>
       <c r="B21" s="4">
@@ -2573,7 +2575,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="11" t="s">
         <v>176</v>
       </c>
       <c r="B22" s="4">
@@ -2602,7 +2604,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="11" t="s">
         <v>177</v>
       </c>
       <c r="B23" s="4">
@@ -2631,7 +2633,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="25" t="s">
         <v>166</v>
       </c>
       <c r="B24" s="4"/>
@@ -2913,7 +2915,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="27" t="s">
         <v>167</v>
       </c>
       <c r="B34" s="5"/>
@@ -3024,7 +3026,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="26" t="s">
         <v>168</v>
       </c>
       <c r="B38" s="6"/>
@@ -3077,7 +3079,7 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="22" t="s">
         <v>442</v>
       </c>
       <c r="B41" s="8">
@@ -3112,7 +3114,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="22" t="s">
         <v>443</v>
       </c>
       <c r="B42" s="8">
@@ -3147,7 +3149,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="22" t="s">
         <v>444</v>
       </c>
       <c r="B43" s="8">
@@ -3182,7 +3184,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="22" t="s">
         <v>445</v>
       </c>
       <c r="B44" s="8">
@@ -3217,7 +3219,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="22" t="s">
         <v>446</v>
       </c>
       <c r="B45" s="8">
@@ -3237,7 +3239,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="22" t="s">
         <v>449</v>
       </c>
       <c r="B46" s="8">
@@ -3257,7 +3259,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="22" t="s">
         <v>450</v>
       </c>
       <c r="B47" s="8">
@@ -3277,7 +3279,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="22" t="s">
         <v>451</v>
       </c>
       <c r="B48" s="8">
@@ -3297,7 +3299,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="22" t="s">
         <v>326</v>
       </c>
       <c r="B49" s="8">
@@ -3335,7 +3337,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="22" t="s">
         <v>200</v>
       </c>
       <c r="B50" s="8">
@@ -3367,11 +3369,11 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="22" t="s">
         <v>201</v>
       </c>
       <c r="B51" s="8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>153</v>
@@ -3402,11 +3404,11 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="27" t="s">
-        <v>327</v>
+      <c r="A52" s="31" t="s">
+        <v>460</v>
       </c>
       <c r="B52" s="8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>0</v>
@@ -3428,60 +3430,57 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="27" t="s">
-        <v>328</v>
+      <c r="A53" s="22" t="s">
+        <v>327</v>
       </c>
       <c r="B53" s="8">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" t="s">
+        <v>189</v>
+      </c>
+      <c r="F53" t="s">
+        <v>202</v>
+      </c>
+      <c r="G53" t="s">
+        <v>203</v>
+      </c>
+      <c r="H53" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="B54" s="8">
+        <v>41</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
         <v>205</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>206</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>207</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="27" t="s">
+    <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="22" t="s">
         <v>297</v>
-      </c>
-      <c r="B54" s="8">
-        <v>42</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54">
-        <v>2017</v>
-      </c>
-      <c r="E54">
-        <v>2018</v>
-      </c>
-      <c r="F54">
-        <v>2019</v>
-      </c>
-      <c r="G54">
-        <v>2020</v>
-      </c>
-      <c r="H54">
-        <v>2021</v>
-      </c>
-      <c r="I54">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
-        <v>298</v>
       </c>
       <c r="B55" s="8">
         <v>42</v>
@@ -3509,11 +3508,11 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="27" t="s">
-        <v>305</v>
+      <c r="A56" s="13" t="s">
+        <v>298</v>
       </c>
       <c r="B56" s="8">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>153</v>
@@ -3538,8 +3537,8 @@
       </c>
     </row>
     <row r="57" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
-        <v>299</v>
+      <c r="A57" s="22" t="s">
+        <v>305</v>
       </c>
       <c r="B57" s="8">
         <v>43</v>
@@ -3567,11 +3566,11 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="27" t="s">
-        <v>306</v>
+      <c r="A58" s="13" t="s">
+        <v>299</v>
       </c>
       <c r="B58" s="8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>153</v>
@@ -3596,8 +3595,8 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
-        <v>300</v>
+      <c r="A59" s="22" t="s">
+        <v>306</v>
       </c>
       <c r="B59" s="8">
         <v>44</v>
@@ -3625,11 +3624,11 @@
       </c>
     </row>
     <row r="60" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="27" t="s">
-        <v>307</v>
+      <c r="A60" s="13" t="s">
+        <v>300</v>
       </c>
       <c r="B60" s="8">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>153</v>
@@ -3654,8 +3653,8 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
-        <v>301</v>
+      <c r="A61" s="22" t="s">
+        <v>307</v>
       </c>
       <c r="B61" s="8">
         <v>45</v>
@@ -3683,11 +3682,11 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="27" t="s">
-        <v>310</v>
+      <c r="A62" s="13" t="s">
+        <v>301</v>
       </c>
       <c r="B62" s="8">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>153</v>
@@ -3712,8 +3711,8 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13" t="s">
-        <v>302</v>
+      <c r="A63" s="22" t="s">
+        <v>310</v>
       </c>
       <c r="B63" s="8">
         <v>46</v>
@@ -3741,11 +3740,11 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="27" t="s">
-        <v>309</v>
+      <c r="A64" s="13" t="s">
+        <v>302</v>
       </c>
       <c r="B64" s="8">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>153</v>
@@ -3770,8 +3769,8 @@
       </c>
     </row>
     <row r="65" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
-        <v>303</v>
+      <c r="A65" s="22" t="s">
+        <v>309</v>
       </c>
       <c r="B65" s="8">
         <v>47</v>
@@ -3799,11 +3798,11 @@
       </c>
     </row>
     <row r="66" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="27" t="s">
-        <v>308</v>
+      <c r="A66" s="13" t="s">
+        <v>303</v>
       </c>
       <c r="B66" s="8">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>153</v>
@@ -3828,8 +3827,8 @@
       </c>
     </row>
     <row r="67" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
-        <v>304</v>
+      <c r="A67" s="22" t="s">
+        <v>308</v>
       </c>
       <c r="B67" s="8">
         <v>48</v>
@@ -3857,11 +3856,11 @@
       </c>
     </row>
     <row r="68" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="27" t="s">
-        <v>447</v>
+      <c r="A68" s="13" t="s">
+        <v>304</v>
       </c>
       <c r="B68" s="8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>153</v>
@@ -3886,8 +3885,8 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="27" t="s">
-        <v>448</v>
+      <c r="A69" s="22" t="s">
+        <v>447</v>
       </c>
       <c r="B69" s="8">
         <v>49</v>
@@ -3915,43 +3914,43 @@
       </c>
     </row>
     <row r="70" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="27" t="s">
+      <c r="A70" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="B70" s="8">
+        <v>49</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70">
+        <v>2017</v>
+      </c>
+      <c r="E70">
+        <v>2018</v>
+      </c>
+      <c r="F70">
+        <v>2019</v>
+      </c>
+      <c r="G70">
+        <v>2020</v>
+      </c>
+      <c r="H70">
+        <v>2021</v>
+      </c>
+      <c r="I70">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="22" t="s">
         <v>425</v>
-      </c>
-      <c r="B70" s="8">
-        <v>50</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="D70">
-        <v>2017</v>
-      </c>
-      <c r="E70">
-        <v>2018</v>
-      </c>
-      <c r="F70">
-        <v>2019</v>
-      </c>
-      <c r="G70">
-        <v>2020</v>
-      </c>
-      <c r="H70">
-        <v>2021</v>
-      </c>
-      <c r="I70">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="27" t="s">
-        <v>426</v>
       </c>
       <c r="B71" s="8">
         <v>50</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D71">
         <v>2017</v>
@@ -3973,80 +3972,74 @@
       </c>
     </row>
     <row r="72" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="27" t="s">
-        <v>427</v>
+      <c r="A72" s="22" t="s">
+        <v>426</v>
       </c>
       <c r="B72" s="8">
         <v>50</v>
       </c>
       <c r="C72" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D72">
+        <v>2017</v>
+      </c>
+      <c r="E72">
+        <v>2018</v>
+      </c>
+      <c r="F72">
+        <v>2019</v>
+      </c>
+      <c r="G72">
+        <v>2020</v>
+      </c>
+      <c r="H72">
+        <v>2021</v>
+      </c>
+      <c r="I72">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="22" t="s">
+        <v>427</v>
+      </c>
+      <c r="B73" s="8">
+        <v>50</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D72">
-        <v>2017</v>
-      </c>
-      <c r="E72">
-        <v>2018</v>
-      </c>
-      <c r="F72">
-        <v>2019</v>
-      </c>
-      <c r="G72">
-        <v>2020</v>
-      </c>
-      <c r="H72">
-        <v>2021</v>
-      </c>
-      <c r="I72">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="33" t="s">
+      <c r="D73">
+        <v>2017</v>
+      </c>
+      <c r="E73">
+        <v>2018</v>
+      </c>
+      <c r="F73">
+        <v>2019</v>
+      </c>
+      <c r="G73">
+        <v>2020</v>
+      </c>
+      <c r="H73">
+        <v>2021</v>
+      </c>
+      <c r="I73">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="28" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B74" s="14">
-        <v>51</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>213</v>
-      </c>
-      <c r="E74" t="s">
-        <v>214</v>
-      </c>
-      <c r="F74" t="s">
-        <v>215</v>
-      </c>
-      <c r="G74" t="s">
-        <v>216</v>
-      </c>
-      <c r="H74" t="s">
-        <v>217</v>
-      </c>
-      <c r="I74" t="s">
-        <v>218</v>
-      </c>
-      <c r="J74" t="s">
-        <v>219</v>
-      </c>
-      <c r="K74" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B75" s="14">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>0</v>
@@ -4078,10 +4071,10 @@
     </row>
     <row r="76" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B76" s="14">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>0</v>
@@ -4113,95 +4106,89 @@
     </row>
     <row r="77" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B77" s="14">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>221</v>
+      <c r="D77" t="s">
+        <v>213</v>
       </c>
       <c r="E77" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F77" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G77" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="H77" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="I77" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="J77" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="K77" t="s">
-        <v>228</v>
-      </c>
-      <c r="L77" t="s">
-        <v>229</v>
-      </c>
-      <c r="M77" t="s">
-        <v>230</v>
-      </c>
-      <c r="N77" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B78" s="14">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D78" t="s">
-        <v>232</v>
+      <c r="D78" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="E78" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F78" t="s">
         <v>223</v>
       </c>
       <c r="G78" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H78" t="s">
         <v>225</v>
       </c>
       <c r="I78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J78" t="s">
         <v>227</v>
       </c>
-      <c r="J78" t="s">
-        <v>235</v>
-      </c>
       <c r="K78" t="s">
+        <v>228</v>
+      </c>
+      <c r="L78" t="s">
         <v>229</v>
       </c>
-      <c r="L78" t="s">
-        <v>236</v>
-      </c>
       <c r="M78" t="s">
+        <v>230</v>
+      </c>
+      <c r="N78" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B79" s="14">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>0</v>
@@ -4222,7 +4209,7 @@
         <v>225</v>
       </c>
       <c r="I79" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J79" t="s">
         <v>235</v>
@@ -4239,39 +4226,51 @@
     </row>
     <row r="80" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B80" s="14">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E80" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F80" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="G80" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H80" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I80" t="s">
-        <v>242</v>
+        <v>226</v>
+      </c>
+      <c r="J80" t="s">
+        <v>235</v>
+      </c>
+      <c r="K80" t="s">
+        <v>229</v>
+      </c>
+      <c r="L80" t="s">
+        <v>236</v>
+      </c>
+      <c r="M80" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B81" s="14">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>0</v>
@@ -4283,58 +4282,87 @@
         <v>238</v>
       </c>
       <c r="F81" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G81" t="s">
+        <v>240</v>
+      </c>
+      <c r="H81" t="s">
+        <v>241</v>
+      </c>
+      <c r="I81" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B82" s="14">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D82" t="s">
+        <v>237</v>
+      </c>
+      <c r="E82" t="s">
+        <v>238</v>
+      </c>
+      <c r="F82" t="s">
+        <v>243</v>
+      </c>
+      <c r="G82" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="B83" s="14">
+        <v>59</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
         <v>244</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E83" t="s">
         <v>245</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F83" t="s">
         <v>246</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G83" t="s">
         <v>247</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H83" t="s">
         <v>248</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I83" t="s">
         <v>249</v>
       </c>
-      <c r="J82" t="s">
+      <c r="J83" t="s">
         <v>250</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K83" t="s">
         <v>251</v>
       </c>
-      <c r="L82" t="s">
+      <c r="L83" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="34" t="s">
-        <v>455</v>
-      </c>
-    </row>
     <row r="85" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="34" t="s">
+      <c r="A85" s="29" t="s">
         <v>454</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="29" t="s">
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -4346,15 +4374,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" customWidth="1"/>
     <col min="2" max="2" width="5.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4364,7 +4392,7 @@
       <c r="B1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -4401,7 +4429,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="19" t="s">
         <v>329</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -4459,7 +4487,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="19" t="s">
         <v>296</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -4488,7 +4516,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="16" t="s">
         <v>311</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -4517,7 +4545,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="19" t="s">
         <v>276</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -4656,7 +4684,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="19" t="s">
         <v>284</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -4685,7 +4713,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="16" t="s">
         <v>312</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -4714,7 +4742,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="19" t="s">
         <v>286</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4743,7 +4771,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="16" t="s">
         <v>313</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -4772,7 +4800,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="19" t="s">
         <v>287</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -4801,7 +4829,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="19" t="s">
         <v>288</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -4830,7 +4858,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="19" t="s">
         <v>289</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -4859,7 +4887,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="19" t="s">
         <v>290</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -4894,7 +4922,7 @@
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="20" t="s">
         <v>360</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -5088,7 +5116,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="20" t="s">
         <v>373</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -5117,7 +5145,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="11" t="s">
         <v>374</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -5204,7 +5232,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="20" t="s">
         <v>379</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -5233,7 +5261,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="11" t="s">
         <v>380</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -5401,7 +5429,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="20" t="s">
         <v>392</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -5430,7 +5458,7 @@
       <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="21" t="s">
         <v>394</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -5459,7 +5487,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="21" t="s">
         <v>395</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -5488,7 +5516,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="21" t="s">
         <v>396</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -5517,7 +5545,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="21" t="s">
         <v>398</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -5546,7 +5574,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="21" t="s">
         <v>399</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -5575,7 +5603,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="21" t="s">
         <v>414</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -5593,7 +5621,7 @@
       <c r="F47">
         <v>2019</v>
       </c>
-      <c r="G47" s="20">
+      <c r="G47">
         <v>2020</v>
       </c>
       <c r="H47">
@@ -5604,7 +5632,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="21" t="s">
         <v>401</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -5633,7 +5661,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="21" t="s">
         <v>402</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -5662,7 +5690,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="21" t="s">
         <v>403</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -5691,7 +5719,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="21" t="s">
         <v>404</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -5720,7 +5748,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="21" t="s">
         <v>405</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -5749,7 +5777,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="21" t="s">
         <v>408</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -5778,7 +5806,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="21" t="s">
         <v>409</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -5807,7 +5835,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="30" t="s">
         <v>411</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -5836,7 +5864,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="12" t="s">
         <v>412</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -5865,7 +5893,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="30" t="s">
         <v>417</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -5894,7 +5922,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="12" t="s">
         <v>422</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -5923,7 +5951,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="21" t="s">
         <v>416</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -5952,7 +5980,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="21" t="s">
         <v>418</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -5981,7 +6009,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="21" t="s">
         <v>421</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -6010,7 +6038,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="21" t="s">
         <v>420</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -6039,8 +6067,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="25" t="s">
-        <v>457</v>
+      <c r="A63" s="21" t="s">
+        <v>456</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>423</v>
@@ -6068,8 +6096,8 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="25" t="s">
-        <v>458</v>
+      <c r="A64" s="21" t="s">
+        <v>457</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>423</v>
@@ -6097,8 +6125,8 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="25" t="s">
-        <v>459</v>
+      <c r="A65" s="21" t="s">
+        <v>458</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>428</v>
@@ -6126,8 +6154,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
-        <v>459</v>
+      <c r="A66" s="21" t="s">
+        <v>458</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>428</v>
@@ -6155,7 +6183,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="21" t="s">
         <v>429</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -6184,7 +6212,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="21" t="s">
         <v>431</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -6213,7 +6241,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="21" t="s">
         <v>434</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -6242,7 +6270,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="26" t="s">
+      <c r="A70" s="12" t="s">
         <v>435</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -6271,13 +6299,13 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="27" t="s">
         <v>167</v>
       </c>
       <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="37" t="s">
+      <c r="A72" s="17" t="s">
         <v>438</v>
       </c>
       <c r="B72" s="6" t="s">
@@ -6306,7 +6334,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="37" t="s">
+      <c r="A73" s="17" t="s">
         <v>439</v>
       </c>
       <c r="B73" s="6" t="s">
@@ -6335,7 +6363,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="36" t="s">
+      <c r="A74" s="7" t="s">
         <v>168</v>
       </c>
       <c r="B74" s="6"/>
@@ -6356,21 +6384,20 @@
       <c r="B77" s="14"/>
     </row>
     <row r="78" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="29" t="s">
         <v>453</v>
       </c>
       <c r="B78" s="14"/>
     </row>
     <row r="79" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="34" t="s">
-        <v>456</v>
+      <c r="A79" s="29" t="s">
+        <v>455</v>
       </c>
       <c r="B79" s="14"/>
     </row>
     <row r="80" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15"/>
       <c r="B80" s="14"/>
-      <c r="D80" s="20"/>
     </row>
     <row r="81" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15"/>

</xml_diff>

<commit_message>
updated data overview.xlsx (highlighted duplicated cells)
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FDCEF-EE72-40F4-91CC-7749EA490AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4405AF7C-53B0-4275-B8B3-A7C56016DCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -1607,7 +1607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1639,12 +1639,32 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1976,9 +1996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
-    </sheetView>
+    <sheetView topLeftCell="A46" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3404,7 +3422,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="22" t="s">
         <v>460</v>
       </c>
       <c r="B52" s="8">
@@ -4366,6 +4384,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:Q1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>COUNTIF($D:$Q, D1)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4374,8 +4397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6420,6 +6443,11 @@
       <c r="B85" s="14"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:K1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>COUNTIF($D:$K, D1)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
grouped tables according to type
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4405AF7C-53B0-4275-B8B3-A7C56016DCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB19E46-A3B1-49D5-8BF3-AC2AF77E39E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="475">
   <si>
     <t>Countries</t>
   </si>
@@ -1423,6 +1423,45 @@
   </si>
   <si>
     <t>Tables to be included: 68 (if counting each subtable)</t>
+  </si>
+  <si>
+    <t>Map and time series (c/c-lvl, retrospective)</t>
+  </si>
+  <si>
+    <t>13-20, 26-29, 32</t>
+  </si>
+  <si>
+    <t>42-50</t>
+  </si>
+  <si>
+    <t>1-12, 21-25, 30-31, 33, 36, 39-41, 51-59</t>
+  </si>
+  <si>
+    <t>I-a, I-f, II-a</t>
+  </si>
+  <si>
+    <t>I-b, II-m</t>
+  </si>
+  <si>
+    <t>I-c:d, I-i:p, II-e, II-g, III-a:e, III:h-p, IV-a:b</t>
+  </si>
+  <si>
+    <t>34-35, 37-38</t>
+  </si>
+  <si>
+    <t>Time series only (other/world, retrospective)</t>
+  </si>
+  <si>
+    <t>Other visualization (other/world, snapshot)</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Map only (country/continent-level, snapshot)*</t>
+  </si>
+  <si>
+    <t>*can be augmented with past and future data (then becomes a TS)</t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1596,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1594,6 +1633,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1607,7 +1664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1639,11 +1696,24 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -1994,9 +2064,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4383,9 +4455,46 @@
         <v>461</v>
       </c>
     </row>
+    <row r="88" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="C88" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="C89" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="32" t="s">
+        <v>470</v>
+      </c>
+      <c r="C90" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="33" t="s">
+        <v>471</v>
+      </c>
+      <c r="C91" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>474</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:Q1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>COUNTIF($D:$Q, D1)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4395,10 +4504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A67" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6422,30 +6531,56 @@
       <c r="A80" s="15"/>
       <c r="B80" s="14"/>
     </row>
-    <row r="81" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="15"/>
-      <c r="B81" s="14"/>
-    </row>
-    <row r="82" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="15"/>
-      <c r="B82" s="14"/>
-    </row>
-    <row r="83" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="15"/>
-      <c r="B83" s="14"/>
-    </row>
-    <row r="84" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="15"/>
-      <c r="B84" s="14"/>
-    </row>
-    <row r="85" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="C81" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="C82" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="32" t="s">
+        <v>470</v>
+      </c>
+      <c r="C83" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="33" t="s">
+        <v>471</v>
+      </c>
+      <c r="C84" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15"/>
       <c r="B85" s="14"/>
     </row>
+    <row r="86" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>474</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:K1048576">
+  <conditionalFormatting sqref="D1:K80 D85:K1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>COUNTIF($D:$K, D1)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D81:Q84">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($D:$K, D1)&gt;1</formula>
+      <formula>COUNTIF($D:$Q, D81)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
small fixes of the big update
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8687ABDB-CE2C-4CB2-8F5F-63320FCF18B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44F2B3C-2DA6-49B4-9207-1AE1A962CB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="551">
   <si>
     <t>Countries</t>
   </si>
   <si>
-    <t>Other centres</t>
-  </si>
-  <si>
     <t>Territorial Prelatures</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>Mission stations as share of total pastoral centres</t>
   </si>
   <si>
-    <t>Number of other centres as share of total pastoral centres</t>
-  </si>
-  <si>
     <t>Area in km^2</t>
   </si>
   <si>
@@ -1693,6 +1687,9 @@
   </si>
   <si>
     <t>Other pastoral centres</t>
+  </si>
+  <si>
+    <t>Number of other pastoral centres as share of total pastoral centres</t>
   </si>
 </sst>
 </file>
@@ -2281,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2294,27 +2291,27 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -2323,36 +2320,36 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" t="s">
         <v>184</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>186</v>
       </c>
-      <c r="G3" t="s">
-        <v>188</v>
-      </c>
       <c r="H3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="L3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -2361,51 +2358,51 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" t="s">
         <v>195</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>196</v>
       </c>
-      <c r="F4" t="s">
-        <v>197</v>
-      </c>
-      <c r="G4" t="s">
-        <v>198</v>
-      </c>
       <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>332</v>
+      </c>
+      <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
-        <v>334</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>6</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>8</v>
       </c>
-      <c r="P4" t="s">
-        <v>9</v>
-      </c>
       <c r="Q4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -2414,33 +2411,33 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" t="s">
         <v>199</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>200</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>201</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>202</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>203</v>
       </c>
-      <c r="I5" t="s">
-        <v>204</v>
-      </c>
-      <c r="J5" t="s">
-        <v>205</v>
-      </c>
       <c r="K5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -2449,30 +2446,30 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" t="s">
         <v>175</v>
-      </c>
-      <c r="H6" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
@@ -2481,42 +2478,42 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" t="s">
+        <v>478</v>
+      </c>
+      <c r="F8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" t="s">
         <v>209</v>
       </c>
-      <c r="E8" t="s">
-        <v>480</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>210</v>
       </c>
-      <c r="G8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H8" t="s">
-        <v>212</v>
-      </c>
       <c r="I8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s">
         <v>11</v>
-      </c>
-      <c r="N8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3">
         <v>6</v>
@@ -2525,18 +2522,18 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B10" s="3">
         <v>7</v>
@@ -2545,18 +2542,18 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B11" s="3">
         <v>8</v>
@@ -2565,39 +2562,39 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" t="s">
         <v>218</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>219</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>220</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>221</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>222</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>223</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>224</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>225</v>
-      </c>
-      <c r="L11" t="s">
-        <v>226</v>
-      </c>
-      <c r="M11" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B12" s="3">
         <v>9</v>
@@ -2606,27 +2603,27 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" t="s">
         <v>234</v>
       </c>
-      <c r="E12" t="s">
-        <v>235</v>
-      </c>
-      <c r="F12" t="s">
-        <v>236</v>
-      </c>
       <c r="G12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B13" s="3">
         <v>10</v>
@@ -2635,24 +2632,24 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
+        <v>486</v>
+      </c>
+      <c r="E13" t="s">
+        <v>487</v>
+      </c>
+      <c r="F13" t="s">
+        <v>478</v>
+      </c>
+      <c r="G13" t="s">
         <v>488</v>
       </c>
-      <c r="E13" t="s">
-        <v>489</v>
-      </c>
-      <c r="F13" t="s">
-        <v>480</v>
-      </c>
-      <c r="G13" t="s">
-        <v>490</v>
-      </c>
       <c r="H13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B14" s="3">
         <v>11</v>
@@ -2661,30 +2658,30 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F14" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G14" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H14" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="J14" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B15" s="3">
         <v>12</v>
@@ -2693,21 +2690,21 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F15" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G15" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B16" s="3">
         <v>13</v>
@@ -2736,7 +2733,7 @@
     </row>
     <row r="17" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B17" s="3">
         <v>14</v>
@@ -2765,7 +2762,7 @@
     </row>
     <row r="18" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B18" s="3">
         <v>15</v>
@@ -2794,7 +2791,7 @@
     </row>
     <row r="19" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B19" s="3">
         <v>16</v>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="20" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B20" s="3">
         <v>17</v>
@@ -2852,7 +2849,7 @@
     </row>
     <row r="21" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B21" s="3">
         <v>18</v>
@@ -2881,7 +2878,7 @@
     </row>
     <row r="22" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B22" s="3">
         <v>19</v>
@@ -2910,7 +2907,7 @@
     </row>
     <row r="23" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B23" s="3">
         <v>20</v>
@@ -2939,13 +2936,13 @@
     </row>
     <row r="24" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="4">
         <v>21</v>
@@ -2954,33 +2951,33 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
+        <v>246</v>
+      </c>
+      <c r="E25" t="s">
+        <v>247</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="H25" t="s">
         <v>248</v>
       </c>
-      <c r="E25" t="s">
+      <c r="I25" t="s">
         <v>249</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G25" s="14" t="s">
+      <c r="J25" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="H25" t="s">
-        <v>250</v>
-      </c>
-      <c r="I25" t="s">
-        <v>251</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>256</v>
-      </c>
       <c r="K25" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="4">
         <v>22</v>
@@ -2989,45 +2986,45 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
+        <v>281</v>
+      </c>
+      <c r="E26" t="s">
+        <v>282</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="G26" t="s">
+        <v>280</v>
+      </c>
+      <c r="H26" t="s">
         <v>283</v>
       </c>
-      <c r="E26" t="s">
+      <c r="I26" t="s">
         <v>284</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="G26" t="s">
-        <v>282</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>285</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>286</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>287</v>
       </c>
-      <c r="K26" t="s">
-        <v>288</v>
-      </c>
-      <c r="L26" t="s">
-        <v>289</v>
-      </c>
       <c r="M26" s="26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N26" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="4">
         <v>23</v>
@@ -3036,18 +3033,18 @@
         <v>0</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="4">
         <v>24</v>
@@ -3056,18 +3053,18 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E28" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="4">
         <v>25</v>
@@ -3076,36 +3073,36 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>296</v>
+      </c>
+      <c r="F29" t="s">
         <v>13</v>
       </c>
-      <c r="E29" t="s">
-        <v>298</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
-      </c>
       <c r="G29" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J29" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K29" t="s">
+        <v>291</v>
+      </c>
+      <c r="L29" t="s">
         <v>293</v>
-      </c>
-      <c r="L29" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B30" s="4">
         <v>26</v>
@@ -3134,7 +3131,7 @@
     </row>
     <row r="31" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B31" s="4">
         <v>27</v>
@@ -3163,7 +3160,7 @@
     </row>
     <row r="32" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B32" s="4">
         <v>28</v>
@@ -3192,7 +3189,7 @@
     </row>
     <row r="33" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B33" s="4">
         <v>29</v>
@@ -3221,13 +3218,13 @@
     </row>
     <row r="34" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="5">
         <v>30</v>
@@ -3236,33 +3233,33 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E35" t="s">
+        <v>298</v>
+      </c>
+      <c r="F35" t="s">
         <v>300</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
+        <v>305</v>
+      </c>
+      <c r="H35" t="s">
         <v>302</v>
       </c>
-      <c r="G35" t="s">
-        <v>307</v>
-      </c>
-      <c r="H35" t="s">
-        <v>304</v>
-      </c>
       <c r="I35" t="s">
+        <v>301</v>
+      </c>
+      <c r="J35" t="s">
         <v>303</v>
       </c>
-      <c r="J35" t="s">
-        <v>305</v>
-      </c>
       <c r="K35" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="5">
         <v>31</v>
@@ -3271,21 +3268,21 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
+        <v>307</v>
+      </c>
+      <c r="E36" t="s">
+        <v>308</v>
+      </c>
+      <c r="F36" t="s">
         <v>309</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>310</v>
-      </c>
-      <c r="F36" t="s">
-        <v>311</v>
-      </c>
-      <c r="G36" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B37" s="5">
         <v>32</v>
@@ -3294,51 +3291,51 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
+        <v>311</v>
+      </c>
+      <c r="E37" t="s">
+        <v>312</v>
+      </c>
+      <c r="F37" t="s">
         <v>313</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>314</v>
       </c>
-      <c r="F37" t="s">
+      <c r="H37" t="s">
         <v>315</v>
       </c>
-      <c r="G37" t="s">
+      <c r="I37" t="s">
         <v>316</v>
       </c>
-      <c r="H37" t="s">
+      <c r="J37" t="s">
         <v>317</v>
       </c>
-      <c r="I37" t="s">
+      <c r="K37" t="s">
         <v>318</v>
       </c>
-      <c r="J37" t="s">
+      <c r="L37" t="s">
         <v>319</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>320</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>321</v>
       </c>
-      <c r="M37" t="s">
+      <c r="O37" t="s">
         <v>322</v>
-      </c>
-      <c r="N37" t="s">
-        <v>323</v>
-      </c>
-      <c r="O37" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="6">
         <v>33</v>
@@ -3347,265 +3344,265 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
         <v>15</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>16</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
+        <v>324</v>
+      </c>
+      <c r="H39" t="s">
+        <v>325</v>
+      </c>
+      <c r="I39" t="s">
         <v>17</v>
       </c>
-      <c r="G39" t="s">
+      <c r="J39" t="s">
         <v>326</v>
       </c>
-      <c r="H39" t="s">
+      <c r="K39" t="s">
         <v>327</v>
       </c>
-      <c r="I39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="L39" t="s">
+        <v>335</v>
+      </c>
+      <c r="M39" t="s">
         <v>328</v>
-      </c>
-      <c r="K39" t="s">
-        <v>329</v>
-      </c>
-      <c r="L39" t="s">
-        <v>337</v>
-      </c>
-      <c r="M39" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="6"/>
     </row>
     <row r="41" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E41" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F41" t="s">
+        <v>336</v>
+      </c>
+      <c r="G41" t="s">
+        <v>337</v>
+      </c>
+      <c r="H41" t="s">
         <v>338</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>339</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>340</v>
       </c>
-      <c r="I41" t="s">
-        <v>341</v>
-      </c>
-      <c r="J41" t="s">
-        <v>342</v>
-      </c>
       <c r="K41" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E42" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F42" t="s">
+        <v>341</v>
+      </c>
+      <c r="G42" t="s">
+        <v>342</v>
+      </c>
+      <c r="H42" t="s">
         <v>343</v>
       </c>
-      <c r="G42" t="s">
+      <c r="I42" t="s">
         <v>344</v>
       </c>
-      <c r="H42" t="s">
+      <c r="J42" t="s">
         <v>345</v>
       </c>
-      <c r="I42" t="s">
-        <v>346</v>
-      </c>
-      <c r="J42" t="s">
-        <v>347</v>
-      </c>
       <c r="K42" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E43" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F43" t="s">
+        <v>346</v>
+      </c>
+      <c r="G43" t="s">
+        <v>347</v>
+      </c>
+      <c r="H43" t="s">
         <v>348</v>
       </c>
-      <c r="G43" t="s">
+      <c r="I43" t="s">
         <v>349</v>
       </c>
-      <c r="H43" t="s">
+      <c r="J43" t="s">
         <v>350</v>
       </c>
-      <c r="I43" t="s">
-        <v>351</v>
-      </c>
-      <c r="J43" t="s">
-        <v>352</v>
-      </c>
       <c r="K43" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E44" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F44" t="s">
+        <v>351</v>
+      </c>
+      <c r="G44" t="s">
+        <v>352</v>
+      </c>
+      <c r="H44" t="s">
         <v>353</v>
       </c>
-      <c r="G44" t="s">
+      <c r="I44" t="s">
         <v>354</v>
       </c>
-      <c r="H44" t="s">
+      <c r="J44" t="s">
         <v>355</v>
       </c>
-      <c r="I44" t="s">
-        <v>356</v>
-      </c>
-      <c r="J44" t="s">
-        <v>357</v>
-      </c>
       <c r="K44" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E45" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F45" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E47" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F47" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E48" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B49" s="7">
         <v>36</v>
@@ -3614,103 +3611,103 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E49" t="s">
+        <v>336</v>
+      </c>
+      <c r="F49" t="s">
+        <v>337</v>
+      </c>
+      <c r="G49" t="s">
         <v>338</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>339</v>
       </c>
-      <c r="G49" t="s">
+      <c r="I49" t="s">
         <v>340</v>
       </c>
-      <c r="H49" t="s">
-        <v>341</v>
-      </c>
-      <c r="I49" t="s">
-        <v>342</v>
-      </c>
       <c r="J49" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="K49" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L49" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B50" s="7">
         <v>37</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E50" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F50" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G50" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H50" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I50" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J50" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B51" s="7">
         <v>38</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E51" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F51" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G51" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H51" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I51" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="J51" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="K51" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B52" s="7">
         <v>39</v>
@@ -3719,24 +3716,24 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E52" t="s">
+        <v>512</v>
+      </c>
+      <c r="F52" t="s">
+        <v>513</v>
+      </c>
+      <c r="G52" t="s">
         <v>514</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>515</v>
-      </c>
-      <c r="G52" t="s">
-        <v>516</v>
-      </c>
-      <c r="H52" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B53" s="7">
         <v>40</v>
@@ -3745,24 +3742,24 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E53" t="s">
+        <v>516</v>
+      </c>
+      <c r="F53" t="s">
+        <v>517</v>
+      </c>
+      <c r="G53" t="s">
         <v>518</v>
       </c>
-      <c r="F53" t="s">
+      <c r="H53" t="s">
         <v>519</v>
-      </c>
-      <c r="G53" t="s">
-        <v>520</v>
-      </c>
-      <c r="H53" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B54" s="7">
         <v>41</v>
@@ -3771,27 +3768,27 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E54" t="s">
+        <v>520</v>
+      </c>
+      <c r="F54" t="s">
+        <v>521</v>
+      </c>
+      <c r="G54" t="s">
         <v>522</v>
-      </c>
-      <c r="F54" t="s">
-        <v>523</v>
-      </c>
-      <c r="G54" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D55">
         <v>2017</v>
@@ -3814,13 +3811,13 @@
     </row>
     <row r="56" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D56">
         <v>2017</v>
@@ -3843,13 +3840,13 @@
     </row>
     <row r="57" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D57">
         <v>2017</v>
@@ -3872,13 +3869,13 @@
     </row>
     <row r="58" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D58">
         <v>2017</v>
@@ -3901,13 +3898,13 @@
     </row>
     <row r="59" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D59">
         <v>2017</v>
@@ -3930,13 +3927,13 @@
     </row>
     <row r="60" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D60">
         <v>2017</v>
@@ -3959,13 +3956,13 @@
     </row>
     <row r="61" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D61">
         <v>2017</v>
@@ -3988,13 +3985,13 @@
     </row>
     <row r="62" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62">
         <v>2017</v>
@@ -4017,13 +4014,13 @@
     </row>
     <row r="63" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D63">
         <v>2017</v>
@@ -4046,13 +4043,13 @@
     </row>
     <row r="64" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D64">
         <v>2017</v>
@@ -4075,13 +4072,13 @@
     </row>
     <row r="65" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D65">
         <v>2017</v>
@@ -4104,13 +4101,13 @@
     </row>
     <row r="66" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D66">
         <v>2017</v>
@@ -4133,13 +4130,13 @@
     </row>
     <row r="67" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D67">
         <v>2017</v>
@@ -4162,13 +4159,13 @@
     </row>
     <row r="68" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D68">
         <v>2017</v>
@@ -4191,13 +4188,13 @@
     </row>
     <row r="69" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D69">
         <v>2017</v>
@@ -4220,13 +4217,13 @@
     </row>
     <row r="70" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D70">
         <v>2017</v>
@@ -4249,13 +4246,13 @@
     </row>
     <row r="71" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D71">
         <v>2017</v>
@@ -4278,13 +4275,13 @@
     </row>
     <row r="72" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D72">
         <v>2017</v>
@@ -4307,13 +4304,13 @@
     </row>
     <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D73">
         <v>2017</v>
@@ -4336,12 +4333,12 @@
     </row>
     <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B75" s="10">
         <v>51</v>
@@ -4350,33 +4347,33 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
+        <v>398</v>
+      </c>
+      <c r="E75" t="s">
+        <v>399</v>
+      </c>
+      <c r="F75" t="s">
         <v>400</v>
       </c>
-      <c r="E75" t="s">
+      <c r="G75" t="s">
         <v>401</v>
       </c>
-      <c r="F75" t="s">
+      <c r="H75" t="s">
         <v>402</v>
       </c>
-      <c r="G75" t="s">
+      <c r="I75" t="s">
         <v>403</v>
       </c>
-      <c r="H75" t="s">
+      <c r="J75" t="s">
         <v>404</v>
       </c>
-      <c r="I75" t="s">
+      <c r="K75" t="s">
         <v>405</v>
-      </c>
-      <c r="J75" t="s">
-        <v>406</v>
-      </c>
-      <c r="K75" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B76" s="10">
         <v>52</v>
@@ -4385,33 +4382,33 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
+        <v>406</v>
+      </c>
+      <c r="E76" t="s">
+        <v>407</v>
+      </c>
+      <c r="F76" t="s">
         <v>408</v>
       </c>
-      <c r="E76" t="s">
+      <c r="G76" t="s">
         <v>409</v>
       </c>
-      <c r="F76" t="s">
+      <c r="H76" t="s">
         <v>410</v>
       </c>
-      <c r="G76" t="s">
+      <c r="I76" t="s">
         <v>411</v>
       </c>
-      <c r="H76" t="s">
+      <c r="J76" t="s">
         <v>412</v>
       </c>
-      <c r="I76" t="s">
+      <c r="K76" t="s">
         <v>413</v>
-      </c>
-      <c r="J76" t="s">
-        <v>414</v>
-      </c>
-      <c r="K76" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B77" s="10">
         <v>53</v>
@@ -4420,33 +4417,33 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
+        <v>414</v>
+      </c>
+      <c r="E77" t="s">
+        <v>415</v>
+      </c>
+      <c r="F77" t="s">
         <v>416</v>
       </c>
-      <c r="E77" t="s">
+      <c r="G77" t="s">
         <v>417</v>
       </c>
-      <c r="F77" t="s">
+      <c r="H77" t="s">
         <v>418</v>
       </c>
-      <c r="G77" t="s">
+      <c r="I77" t="s">
         <v>419</v>
       </c>
-      <c r="H77" t="s">
+      <c r="J77" t="s">
         <v>420</v>
       </c>
-      <c r="I77" t="s">
+      <c r="K77" t="s">
         <v>421</v>
-      </c>
-      <c r="J77" t="s">
-        <v>422</v>
-      </c>
-      <c r="K77" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B78" s="10">
         <v>54</v>
@@ -4455,42 +4452,42 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
+        <v>422</v>
+      </c>
+      <c r="E78" t="s">
+        <v>423</v>
+      </c>
+      <c r="F78" t="s">
         <v>424</v>
       </c>
-      <c r="E78" t="s">
+      <c r="G78" t="s">
         <v>425</v>
       </c>
-      <c r="F78" t="s">
-        <v>426</v>
-      </c>
-      <c r="G78" t="s">
-        <v>427</v>
-      </c>
       <c r="H78" t="s">
+        <v>437</v>
+      </c>
+      <c r="I78" t="s">
+        <v>436</v>
+      </c>
+      <c r="J78" t="s">
+        <v>432</v>
+      </c>
+      <c r="K78" t="s">
+        <v>433</v>
+      </c>
+      <c r="L78" t="s">
+        <v>434</v>
+      </c>
+      <c r="M78" t="s">
+        <v>435</v>
+      </c>
+      <c r="N78" t="s">
         <v>439</v>
-      </c>
-      <c r="I78" t="s">
-        <v>438</v>
-      </c>
-      <c r="J78" t="s">
-        <v>434</v>
-      </c>
-      <c r="K78" t="s">
-        <v>435</v>
-      </c>
-      <c r="L78" t="s">
-        <v>436</v>
-      </c>
-      <c r="M78" t="s">
-        <v>437</v>
-      </c>
-      <c r="N78" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B79" s="10">
         <v>55</v>
@@ -4499,39 +4496,39 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
+        <v>426</v>
+      </c>
+      <c r="E79" t="s">
+        <v>440</v>
+      </c>
+      <c r="F79" t="s">
+        <v>427</v>
+      </c>
+      <c r="G79" t="s">
         <v>428</v>
       </c>
-      <c r="E79" t="s">
+      <c r="H79" t="s">
+        <v>438</v>
+      </c>
+      <c r="I79" t="s">
+        <v>441</v>
+      </c>
+      <c r="J79" t="s">
         <v>442</v>
       </c>
-      <c r="F79" t="s">
-        <v>429</v>
-      </c>
-      <c r="G79" t="s">
-        <v>430</v>
-      </c>
-      <c r="H79" t="s">
-        <v>440</v>
-      </c>
-      <c r="I79" t="s">
+      <c r="K79" t="s">
         <v>443</v>
       </c>
-      <c r="J79" t="s">
+      <c r="L79" t="s">
         <v>444</v>
       </c>
-      <c r="K79" t="s">
+      <c r="M79" t="s">
         <v>445</v>
-      </c>
-      <c r="L79" t="s">
-        <v>446</v>
-      </c>
-      <c r="M79" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B80" s="10">
         <v>56</v>
@@ -4540,39 +4537,39 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
+        <v>429</v>
+      </c>
+      <c r="E80" t="s">
+        <v>446</v>
+      </c>
+      <c r="F80" t="s">
+        <v>430</v>
+      </c>
+      <c r="G80" t="s">
         <v>431</v>
       </c>
-      <c r="E80" t="s">
+      <c r="H80" t="s">
+        <v>447</v>
+      </c>
+      <c r="I80" t="s">
         <v>448</v>
       </c>
-      <c r="F80" t="s">
-        <v>432</v>
-      </c>
-      <c r="G80" t="s">
-        <v>433</v>
-      </c>
-      <c r="H80" t="s">
+      <c r="J80" t="s">
         <v>449</v>
       </c>
-      <c r="I80" t="s">
+      <c r="K80" t="s">
         <v>450</v>
       </c>
-      <c r="J80" t="s">
+      <c r="L80" t="s">
         <v>451</v>
       </c>
-      <c r="K80" t="s">
+      <c r="M80" t="s">
         <v>452</v>
-      </c>
-      <c r="L80" t="s">
-        <v>453</v>
-      </c>
-      <c r="M80" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B81" s="10">
         <v>57</v>
@@ -4581,27 +4578,27 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
+        <v>453</v>
+      </c>
+      <c r="E81" t="s">
+        <v>454</v>
+      </c>
+      <c r="F81" t="s">
         <v>455</v>
       </c>
-      <c r="E81" t="s">
+      <c r="G81" t="s">
         <v>456</v>
       </c>
-      <c r="F81" t="s">
+      <c r="H81" t="s">
         <v>457</v>
       </c>
-      <c r="G81" t="s">
+      <c r="I81" t="s">
         <v>458</v>
-      </c>
-      <c r="H81" t="s">
-        <v>459</v>
-      </c>
-      <c r="I81" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B82" s="10">
         <v>58</v>
@@ -4610,21 +4607,21 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
+        <v>459</v>
+      </c>
+      <c r="E82" t="s">
+        <v>460</v>
+      </c>
+      <c r="F82" t="s">
         <v>461</v>
       </c>
-      <c r="E82" t="s">
+      <c r="G82" t="s">
         <v>462</v>
-      </c>
-      <c r="F82" t="s">
-        <v>463</v>
-      </c>
-      <c r="G82" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B83" s="10">
         <v>59</v>
@@ -4633,68 +4630,68 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
+        <v>463</v>
+      </c>
+      <c r="E83" t="s">
+        <v>464</v>
+      </c>
+      <c r="F83" t="s">
         <v>465</v>
       </c>
-      <c r="E83" t="s">
+      <c r="G83" t="s">
         <v>466</v>
       </c>
-      <c r="F83" t="s">
+      <c r="H83" t="s">
         <v>467</v>
       </c>
-      <c r="G83" t="s">
+      <c r="I83" t="s">
         <v>468</v>
       </c>
-      <c r="H83" t="s">
+      <c r="J83" t="s">
+        <v>470</v>
+      </c>
+      <c r="K83" t="s">
+        <v>471</v>
+      </c>
+      <c r="L83" t="s">
         <v>469</v>
-      </c>
-      <c r="I83" t="s">
-        <v>470</v>
-      </c>
-      <c r="J83" t="s">
-        <v>472</v>
-      </c>
-      <c r="K83" t="s">
-        <v>473</v>
-      </c>
-      <c r="L83" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" t="s">
         <v>87</v>
-      </c>
-      <c r="C87" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -4710,8 +4707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4723,114 +4720,114 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>184</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>186</v>
-      </c>
       <c r="G3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
         <v>68</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
         <v>71</v>
       </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>72</v>
-      </c>
-      <c r="I4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>71</v>
       </c>
-      <c r="G5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>72</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <v>2017</v>
@@ -4853,13 +4850,13 @@
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>2017</v>
@@ -4882,13 +4879,13 @@
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>2017</v>
@@ -4911,59 +4908,59 @@
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
-      </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" t="s">
         <v>175</v>
-      </c>
-      <c r="G10" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11">
         <v>2017</v>
@@ -4986,48 +4983,48 @@
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" t="s">
         <v>180</v>
       </c>
-      <c r="F12" t="s">
-        <v>190</v>
-      </c>
-      <c r="G12" t="s">
-        <v>181</v>
-      </c>
       <c r="H12" t="s">
-        <v>1</v>
+        <v>549</v>
       </c>
       <c r="I12" t="s">
-        <v>182</v>
+        <v>550</v>
       </c>
       <c r="J12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>2017</v>
@@ -5050,13 +5047,13 @@
     </row>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>2017</v>
@@ -5079,13 +5076,13 @@
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>2017</v>
@@ -5108,13 +5105,13 @@
     </row>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>2017</v>
@@ -5137,13 +5134,13 @@
     </row>
     <row r="17" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17">
         <v>2017</v>
@@ -5166,13 +5163,13 @@
     </row>
     <row r="18" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>2017</v>
@@ -5195,13 +5192,13 @@
     </row>
     <row r="19" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>2017</v>
@@ -5224,13 +5221,13 @@
     </row>
     <row r="20" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20">
         <v>2017</v>
@@ -5253,39 +5250,39 @@
     </row>
     <row r="21" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>481</v>
+      </c>
+      <c r="E22" t="s">
         <v>482</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>483</v>
-      </c>
-      <c r="E22" t="s">
-        <v>484</v>
-      </c>
       <c r="F22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23">
         <v>2017</v>
@@ -5308,13 +5305,13 @@
     </row>
     <row r="24" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24">
         <v>2017</v>
@@ -5337,13 +5334,13 @@
     </row>
     <row r="25" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>2017</v>
@@ -5366,13 +5363,13 @@
     </row>
     <row r="26" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26">
         <v>2017</v>
@@ -5395,13 +5392,13 @@
     </row>
     <row r="27" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27">
         <v>2017</v>
@@ -5424,13 +5421,13 @@
     </row>
     <row r="28" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28">
         <v>2017</v>
@@ -5453,13 +5450,13 @@
     </row>
     <row r="29" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29">
         <v>2017</v>
@@ -5482,13 +5479,13 @@
     </row>
     <row r="30" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <v>2017</v>
@@ -5511,13 +5508,13 @@
     </row>
     <row r="31" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <v>2017</v>
@@ -5540,13 +5537,13 @@
     </row>
     <row r="32" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32">
         <v>2017</v>
@@ -5569,13 +5566,13 @@
     </row>
     <row r="33" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33">
         <v>2017</v>
@@ -5598,13 +5595,13 @@
     </row>
     <row r="34" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34">
         <v>2017</v>
@@ -5627,13 +5624,13 @@
     </row>
     <row r="35" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35">
         <v>2017</v>
@@ -5656,13 +5653,13 @@
     </row>
     <row r="36" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36">
         <v>2017</v>
@@ -5685,13 +5682,13 @@
     </row>
     <row r="37" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37">
         <v>2017</v>
@@ -5714,13 +5711,13 @@
     </row>
     <row r="38" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38">
         <v>2017</v>
@@ -5743,65 +5740,65 @@
     </row>
     <row r="39" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E39" t="s">
+        <v>526</v>
+      </c>
+      <c r="F39" t="s">
         <v>528</v>
       </c>
-      <c r="F39" t="s">
-        <v>530</v>
-      </c>
       <c r="G39" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="D40" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E40" t="s">
+        <v>526</v>
+      </c>
+      <c r="F40" t="s">
         <v>528</v>
       </c>
-      <c r="F40" t="s">
-        <v>530</v>
-      </c>
       <c r="G40" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42">
         <v>2017</v>
@@ -5824,13 +5821,13 @@
     </row>
     <row r="43" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43">
         <v>2017</v>
@@ -5853,13 +5850,13 @@
     </row>
     <row r="44" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44">
         <v>2017</v>
@@ -5882,13 +5879,13 @@
     </row>
     <row r="45" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45">
         <v>2017</v>
@@ -5911,13 +5908,13 @@
     </row>
     <row r="46" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46">
         <v>2017</v>
@@ -5940,13 +5937,13 @@
     </row>
     <row r="47" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47">
         <v>2017</v>
@@ -5969,13 +5966,13 @@
     </row>
     <row r="48" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48">
         <v>2017</v>
@@ -5998,13 +5995,13 @@
     </row>
     <row r="49" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49">
         <v>2017</v>
@@ -6027,13 +6024,13 @@
     </row>
     <row r="50" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50">
         <v>2017</v>
@@ -6056,13 +6053,13 @@
     </row>
     <row r="51" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -6085,13 +6082,13 @@
     </row>
     <row r="52" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52">
         <v>2017</v>
@@ -6114,13 +6111,13 @@
     </row>
     <row r="53" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D53">
         <v>2017</v>
@@ -6143,13 +6140,13 @@
     </row>
     <row r="54" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54">
         <v>2017</v>
@@ -6172,13 +6169,13 @@
     </row>
     <row r="55" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55">
         <v>2017</v>
@@ -6201,13 +6198,13 @@
     </row>
     <row r="56" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D56">
         <v>2017</v>
@@ -6230,13 +6227,13 @@
     </row>
     <row r="57" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="25" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57">
         <v>2017</v>
@@ -6259,13 +6256,13 @@
     </row>
     <row r="58" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="25" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58">
         <v>2017</v>
@@ -6288,13 +6285,13 @@
     </row>
     <row r="59" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D59">
         <v>2017</v>
@@ -6317,13 +6314,13 @@
     </row>
     <row r="60" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D60">
         <v>2017</v>
@@ -6346,13 +6343,13 @@
     </row>
     <row r="61" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D61">
         <v>2017</v>
@@ -6375,13 +6372,13 @@
     </row>
     <row r="62" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D62">
         <v>2017</v>
@@ -6404,13 +6401,13 @@
     </row>
     <row r="63" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D63">
         <v>2017</v>
@@ -6433,13 +6430,13 @@
     </row>
     <row r="64" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D64">
         <v>2017</v>
@@ -6462,13 +6459,13 @@
     </row>
     <row r="65" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D65">
         <v>2017</v>
@@ -6491,13 +6488,13 @@
     </row>
     <row r="66" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D66">
         <v>2017</v>
@@ -6520,13 +6517,13 @@
     </row>
     <row r="67" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67">
         <v>2017</v>
@@ -6549,13 +6546,13 @@
     </row>
     <row r="68" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="27" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68">
         <v>2017</v>
@@ -6578,13 +6575,13 @@
     </row>
     <row r="69" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69">
         <v>2017</v>
@@ -6607,48 +6604,48 @@
     </row>
     <row r="70" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D70" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>296</v>
+      </c>
+      <c r="F70" t="s">
         <v>13</v>
       </c>
-      <c r="E70" t="s">
-        <v>298</v>
-      </c>
-      <c r="F70" t="s">
-        <v>14</v>
-      </c>
       <c r="G70" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H70" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I70" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D72">
         <v>2017</v>
@@ -6671,13 +6668,13 @@
     </row>
     <row r="73" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D73">
         <v>2017</v>
@@ -6700,19 +6697,19 @@
     </row>
     <row r="74" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B75" s="6"/>
     </row>
     <row r="76" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -6725,34 +6722,34 @@
     </row>
     <row r="79" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" t="s">
         <v>95</v>
-      </c>
-      <c r="C81" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -6761,7 +6758,7 @@
     </row>
     <row r="84" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
table numbers converted to text
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44F2B3C-2DA6-49B4-9207-1AE1A962CB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7118FA03-ABBE-4A5F-80B2-0E6026C36E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="560">
   <si>
     <t>Countries</t>
   </si>
@@ -1690,6 +1690,33 @@
   </si>
   <si>
     <t>Number of other pastoral centres as share of total pastoral centres</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
   </si>
 </sst>
 </file>
@@ -1901,7 +1928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1931,6 +1958,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2278,14 +2314,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" style="36" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2293,7 +2327,7 @@
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2307,14 +2341,14 @@
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
+      <c r="B3" s="30" t="s">
+        <v>551</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>0</v>
@@ -2351,8 +2385,8 @@
       <c r="A4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="2">
-        <v>2</v>
+      <c r="B4" s="30" t="s">
+        <v>552</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>0</v>
@@ -2404,8 +2438,8 @@
       <c r="A5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="2">
-        <v>3</v>
+      <c r="B5" s="30" t="s">
+        <v>553</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>0</v>
@@ -2439,8 +2473,8 @@
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2">
-        <v>4</v>
+      <c r="B6" s="30" t="s">
+        <v>554</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>0</v>
@@ -2465,14 +2499,14 @@
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="31"/>
     </row>
     <row r="8" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="3">
-        <v>5</v>
+      <c r="B8" s="31" t="s">
+        <v>555</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>0</v>
@@ -2515,8 +2549,8 @@
       <c r="A9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3">
-        <v>6</v>
+      <c r="B9" s="31" t="s">
+        <v>556</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>0</v>
@@ -2535,8 +2569,8 @@
       <c r="A10" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="3">
-        <v>7</v>
+      <c r="B10" s="31" t="s">
+        <v>557</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>0</v>
@@ -2555,8 +2589,8 @@
       <c r="A11" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="B11" s="3">
-        <v>8</v>
+      <c r="B11" s="31" t="s">
+        <v>558</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>0</v>
@@ -2596,8 +2630,8 @@
       <c r="A12" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="B12" s="3">
-        <v>9</v>
+      <c r="B12" s="31" t="s">
+        <v>559</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
@@ -2625,7 +2659,7 @@
       <c r="A13" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="31">
         <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -2651,7 +2685,7 @@
       <c r="A14" s="17" t="s">
         <v>540</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="31">
         <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -2683,7 +2717,7 @@
       <c r="A15" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="31">
         <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -2706,7 +2740,7 @@
       <c r="A16" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="31">
         <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -2735,7 +2769,7 @@
       <c r="A17" s="17" t="s">
         <v>478</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="31">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -2764,7 +2798,7 @@
       <c r="A18" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="31">
         <v>15</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -2793,7 +2827,7 @@
       <c r="A19" s="17" t="s">
         <v>535</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="31">
         <v>16</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -2822,7 +2856,7 @@
       <c r="A20" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="31">
         <v>17</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -2851,7 +2885,7 @@
       <c r="A21" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="31">
         <v>18</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -2880,7 +2914,7 @@
       <c r="A22" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="31">
         <v>19</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -2909,7 +2943,7 @@
       <c r="A23" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="31">
         <v>20</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -2938,13 +2972,13 @@
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="32">
         <v>21</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -2979,7 +3013,7 @@
       <c r="A26" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="32">
         <v>22</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -3026,7 +3060,7 @@
       <c r="A27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="32">
         <v>23</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -3046,7 +3080,7 @@
       <c r="A28" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="32">
         <v>24</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -3066,7 +3100,7 @@
       <c r="A29" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="32">
         <v>25</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -3104,7 +3138,7 @@
       <c r="A30" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="32">
         <v>26</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -3133,7 +3167,7 @@
       <c r="A31" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="32">
         <v>27</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -3162,7 +3196,7 @@
       <c r="A32" s="25" t="s">
         <v>276</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="32">
         <v>28</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -3191,7 +3225,7 @@
       <c r="A33" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="32">
         <v>29</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -3220,13 +3254,13 @@
       <c r="A34" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="32"/>
     </row>
     <row r="35" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="33">
         <v>30</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -3261,7 +3295,7 @@
       <c r="A36" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="33">
         <v>31</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -3284,7 +3318,7 @@
       <c r="A37" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="33">
         <v>32</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -3331,13 +3365,13 @@
       <c r="A38" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="33"/>
     </row>
     <row r="39" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="34">
         <v>33</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -3378,13 +3412,13 @@
       <c r="A40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="6"/>
+      <c r="B40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="35" t="s">
         <v>147</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -3419,7 +3453,7 @@
       <c r="A42" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="35" t="s">
         <v>148</v>
       </c>
       <c r="C42" s="9" t="s">
@@ -3454,7 +3488,7 @@
       <c r="A43" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="35" t="s">
         <v>149</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -3489,7 +3523,7 @@
       <c r="A44" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="35" t="s">
         <v>150</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -3524,7 +3558,7 @@
       <c r="A45" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="35" t="s">
         <v>151</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -3544,7 +3578,7 @@
       <c r="A46" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C46" s="9" t="s">
@@ -3564,7 +3598,7 @@
       <c r="A47" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="35" t="s">
         <v>153</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -3584,7 +3618,7 @@
       <c r="A48" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="35" t="s">
         <v>154</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -3604,7 +3638,7 @@
       <c r="A49" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="35">
         <v>36</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -3642,7 +3676,7 @@
       <c r="A50" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="35">
         <v>37</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -3674,7 +3708,7 @@
       <c r="A51" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="35">
         <v>38</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -3709,7 +3743,7 @@
       <c r="A52" s="20" t="s">
         <v>385</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="35">
         <v>39</v>
       </c>
       <c r="C52" s="8" t="s">
@@ -3735,7 +3769,7 @@
       <c r="A53" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="35">
         <v>40</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -3761,7 +3795,7 @@
       <c r="A54" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="35">
         <v>41</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -3784,7 +3818,7 @@
       <c r="A55" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="35" t="s">
         <v>155</v>
       </c>
       <c r="C55" s="9" t="s">
@@ -3813,7 +3847,7 @@
       <c r="A56" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="35" t="s">
         <v>156</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -3842,7 +3876,7 @@
       <c r="A57" s="20" t="s">
         <v>545</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="35" t="s">
         <v>157</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -3871,7 +3905,7 @@
       <c r="A58" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="35" t="s">
         <v>158</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -3900,7 +3934,7 @@
       <c r="A59" s="20" t="s">
         <v>533</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="35" t="s">
         <v>159</v>
       </c>
       <c r="C59" s="9" t="s">
@@ -3929,7 +3963,7 @@
       <c r="A60" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="35" t="s">
         <v>160</v>
       </c>
       <c r="C60" s="9" t="s">
@@ -3958,7 +3992,7 @@
       <c r="A61" s="20" t="s">
         <v>538</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="35" t="s">
         <v>161</v>
       </c>
       <c r="C61" s="9" t="s">
@@ -3987,7 +4021,7 @@
       <c r="A62" s="20" t="s">
         <v>539</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="35" t="s">
         <v>162</v>
       </c>
       <c r="C62" s="9" t="s">
@@ -4016,7 +4050,7 @@
       <c r="A63" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="35" t="s">
         <v>163</v>
       </c>
       <c r="C63" s="9" t="s">
@@ -4045,7 +4079,7 @@
       <c r="A64" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="35" t="s">
         <v>164</v>
       </c>
       <c r="C64" s="9" t="s">
@@ -4074,7 +4108,7 @@
       <c r="A65" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="35" t="s">
         <v>165</v>
       </c>
       <c r="C65" s="9" t="s">
@@ -4103,7 +4137,7 @@
       <c r="A66" s="20" t="s">
         <v>392</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -4132,7 +4166,7 @@
       <c r="A67" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="35" t="s">
         <v>167</v>
       </c>
       <c r="C67" s="9" t="s">
@@ -4161,7 +4195,7 @@
       <c r="A68" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="35" t="s">
         <v>168</v>
       </c>
       <c r="C68" s="9" t="s">
@@ -4190,7 +4224,7 @@
       <c r="A69" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="35" t="s">
         <v>169</v>
       </c>
       <c r="C69" s="9" t="s">
@@ -4219,7 +4253,7 @@
       <c r="A70" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="35" t="s">
         <v>170</v>
       </c>
       <c r="C70" s="9" t="s">
@@ -4248,7 +4282,7 @@
       <c r="A71" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="35" t="s">
         <v>171</v>
       </c>
       <c r="C71" s="9" t="s">
@@ -4277,7 +4311,7 @@
       <c r="A72" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="35" t="s">
         <v>172</v>
       </c>
       <c r="C72" s="9" t="s">
@@ -4306,7 +4340,7 @@
       <c r="A73" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="35" t="s">
         <v>173</v>
       </c>
       <c r="C73" s="9" t="s">
@@ -4340,7 +4374,7 @@
       <c r="A75" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="B75" s="10">
+      <c r="B75" s="37">
         <v>51</v>
       </c>
       <c r="C75" s="8" t="s">
@@ -4375,7 +4409,7 @@
       <c r="A76" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="B76" s="10">
+      <c r="B76" s="37">
         <v>52</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -4410,7 +4444,7 @@
       <c r="A77" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="37">
         <v>53</v>
       </c>
       <c r="C77" s="8" t="s">
@@ -4445,7 +4479,7 @@
       <c r="A78" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="10">
+      <c r="B78" s="37">
         <v>54</v>
       </c>
       <c r="C78" s="8" t="s">
@@ -4489,7 +4523,7 @@
       <c r="A79" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" s="37">
         <v>55</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -4530,7 +4564,7 @@
       <c r="A80" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="37">
         <v>56</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -4571,7 +4605,7 @@
       <c r="A81" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" s="37">
         <v>57</v>
       </c>
       <c r="C81" s="8" t="s">
@@ -4600,7 +4634,7 @@
       <c r="A82" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="37">
         <v>58</v>
       </c>
       <c r="C82" s="8" t="s">
@@ -4623,7 +4657,7 @@
       <c r="A83" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="37">
         <v>59</v>
       </c>
       <c r="C83" s="8" t="s">
@@ -4700,6 +4734,9 @@
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -4707,14 +4744,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" style="36" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4722,7 +4759,7 @@
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4736,13 +4773,13 @@
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -4765,7 +4802,7 @@
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="30" t="s">
         <v>98</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4794,7 +4831,7 @@
       <c r="A5" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="30" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -4823,7 +4860,7 @@
       <c r="A6" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -4852,7 +4889,7 @@
       <c r="A7" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -4881,7 +4918,7 @@
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -4910,7 +4947,7 @@
       <c r="A9" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="30" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -4933,7 +4970,7 @@
       <c r="A10" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="30" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -4956,7 +4993,7 @@
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="30" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -4985,7 +5022,7 @@
       <c r="A12" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="30" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -5020,7 +5057,7 @@
       <c r="A13" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="30" t="s">
         <v>102</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -5049,7 +5086,7 @@
       <c r="A14" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="30" t="s">
         <v>103</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -5078,7 +5115,7 @@
       <c r="A15" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="30" t="s">
         <v>104</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -5107,7 +5144,7 @@
       <c r="A16" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="30" t="s">
         <v>105</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -5136,7 +5173,7 @@
       <c r="A17" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="30" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -5165,7 +5202,7 @@
       <c r="A18" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="30" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -5194,7 +5231,7 @@
       <c r="A19" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -5223,7 +5260,7 @@
       <c r="A20" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="30" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -5252,13 +5289,13 @@
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>480</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="31" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -5278,7 +5315,7 @@
       <c r="A23" s="17" t="s">
         <v>483</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="31" t="s">
         <v>106</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -5307,7 +5344,7 @@
       <c r="A24" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="31" t="s">
         <v>107</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -5336,7 +5373,7 @@
       <c r="A25" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="31" t="s">
         <v>108</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5365,7 +5402,7 @@
       <c r="A26" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="31" t="s">
         <v>109</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -5394,7 +5431,7 @@
       <c r="A27" s="17" t="s">
         <v>478</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="31" t="s">
         <v>110</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -5423,7 +5460,7 @@
       <c r="A28" s="17" t="s">
         <v>479</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="31" t="s">
         <v>111</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -5452,7 +5489,7 @@
       <c r="A29" s="17" t="s">
         <v>486</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="31" t="s">
         <v>112</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -5481,7 +5518,7 @@
       <c r="A30" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="31" t="s">
         <v>113</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -5510,7 +5547,7 @@
       <c r="A31" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="31" t="s">
         <v>114</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -5539,7 +5576,7 @@
       <c r="A32" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="31" t="s">
         <v>115</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -5568,7 +5605,7 @@
       <c r="A33" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="31" t="s">
         <v>116</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -5597,7 +5634,7 @@
       <c r="A34" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="31" t="s">
         <v>117</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -5626,7 +5663,7 @@
       <c r="A35" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="31" t="s">
         <v>118</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -5655,7 +5692,7 @@
       <c r="A36" s="17" t="s">
         <v>490</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="31" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -5684,7 +5721,7 @@
       <c r="A37" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="31" t="s">
         <v>120</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -5713,7 +5750,7 @@
       <c r="A38" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="31" t="s">
         <v>121</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -5742,7 +5779,7 @@
       <c r="A39" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="31" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -5765,7 +5802,7 @@
       <c r="A40" s="17" t="s">
         <v>529</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="31" t="s">
         <v>77</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -5788,13 +5825,13 @@
       <c r="A41" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="31"/>
     </row>
     <row r="42" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="32" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="8" t="s">
@@ -5823,7 +5860,7 @@
       <c r="A43" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="32" t="s">
         <v>123</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -5852,7 +5889,7 @@
       <c r="A44" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="32" t="s">
         <v>124</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -5881,7 +5918,7 @@
       <c r="A45" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="32" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -5910,7 +5947,7 @@
       <c r="A46" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="32" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -5939,7 +5976,7 @@
       <c r="A47" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="32" t="s">
         <v>127</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -5968,7 +6005,7 @@
       <c r="A48" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="32" t="s">
         <v>128</v>
       </c>
       <c r="C48" s="8" t="s">
@@ -5997,7 +6034,7 @@
       <c r="A49" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="32" t="s">
         <v>129</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -6026,7 +6063,7 @@
       <c r="A50" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="32" t="s">
         <v>130</v>
       </c>
       <c r="C50" s="8" t="s">
@@ -6055,7 +6092,7 @@
       <c r="A51" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="32" t="s">
         <v>131</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -6084,7 +6121,7 @@
       <c r="A52" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="32" t="s">
         <v>132</v>
       </c>
       <c r="C52" s="8" t="s">
@@ -6113,7 +6150,7 @@
       <c r="A53" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -6142,7 +6179,7 @@
       <c r="A54" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="32" t="s">
         <v>134</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -6171,7 +6208,7 @@
       <c r="A55" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="32" t="s">
         <v>135</v>
       </c>
       <c r="C55" s="8" t="s">
@@ -6200,7 +6237,7 @@
       <c r="A56" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="32" t="s">
         <v>136</v>
       </c>
       <c r="C56" s="8" t="s">
@@ -6229,7 +6266,7 @@
       <c r="A57" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="32" t="s">
         <v>137</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -6258,7 +6295,7 @@
       <c r="A58" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="32" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="8" t="s">
@@ -6287,7 +6324,7 @@
       <c r="A59" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="32" t="s">
         <v>139</v>
       </c>
       <c r="C59" s="8" t="s">
@@ -6316,7 +6353,7 @@
       <c r="A60" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="32" t="s">
         <v>140</v>
       </c>
       <c r="C60" s="8" t="s">
@@ -6345,7 +6382,7 @@
       <c r="A61" s="25" t="s">
         <v>276</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -6374,7 +6411,7 @@
       <c r="A62" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="32" t="s">
         <v>142</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -6403,7 +6440,7 @@
       <c r="A63" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="32" t="s">
         <v>143</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -6432,7 +6469,7 @@
       <c r="A64" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -6461,7 +6498,7 @@
       <c r="A65" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="32" t="s">
         <v>145</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -6490,7 +6527,7 @@
       <c r="A66" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="32" t="s">
         <v>146</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -6519,7 +6556,7 @@
       <c r="A67" s="18" t="s">
         <v>525</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="32" t="s">
         <v>79</v>
       </c>
       <c r="C67" s="8" t="s">
@@ -6548,7 +6585,7 @@
       <c r="A68" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="32" t="s">
         <v>80</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -6577,7 +6614,7 @@
       <c r="A69" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="32" t="s">
         <v>81</v>
       </c>
       <c r="C69" s="8" t="s">
@@ -6606,7 +6643,7 @@
       <c r="A70" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="32" t="s">
         <v>82</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -6635,13 +6672,13 @@
       <c r="A71" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B71" s="4"/>
+      <c r="B71" s="32"/>
     </row>
     <row r="72" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="33" t="s">
         <v>84</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -6670,7 +6707,7 @@
       <c r="A73" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="33" t="s">
         <v>83</v>
       </c>
       <c r="C73" s="8" t="s">
@@ -6699,13 +6736,13 @@
       <c r="A74" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B74" s="5"/>
+      <c r="B74" s="33"/>
     </row>
     <row r="75" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="34"/>
     </row>
     <row r="76" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
@@ -6714,11 +6751,11 @@
     </row>
     <row r="77" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11"/>
-      <c r="B77" s="10"/>
+      <c r="B77" s="37"/>
     </row>
     <row r="78" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11"/>
-      <c r="B78" s="10"/>
+      <c r="B78" s="37"/>
     </row>
     <row r="79" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -6754,7 +6791,7 @@
     </row>
     <row r="83" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11"/>
-      <c r="B83" s="10"/>
+      <c r="B83" s="37"/>
     </row>
     <row r="84" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">

</xml_diff>

<commit_message>
removed notes at the end
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7118FA03-ABBE-4A5F-80B2-0E6026C36E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FCEE04-CD34-4AB6-92CF-8E57B87D82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="547">
   <si>
     <t>Countries</t>
   </si>
@@ -297,42 +297,6 @@
     <t>COLUMNS…</t>
   </si>
   <si>
-    <t>Map and time series (c/c-lvl, retrospective)</t>
-  </si>
-  <si>
-    <t>13-20, 26-29, 32</t>
-  </si>
-  <si>
-    <t>42-50</t>
-  </si>
-  <si>
-    <t>1-12, 21-25, 30-31, 33, 36, 39-41, 51-59</t>
-  </si>
-  <si>
-    <t>I-a, I-f, II-a</t>
-  </si>
-  <si>
-    <t>I-b, II-m</t>
-  </si>
-  <si>
-    <t>I-c:d, I-i:p, II-e, II-g, III-a:e, III:h-p, IV-a:b</t>
-  </si>
-  <si>
-    <t>34-35, 37-38</t>
-  </si>
-  <si>
-    <t>Time series only (other/world, retrospective)</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>Map only (country/continent-level, snapshot)*</t>
-  </si>
-  <si>
-    <t>*can be augmented with past and future data (then becomes a TS)</t>
-  </si>
-  <si>
     <t>I-b-1</t>
   </si>
   <si>
@@ -796,9 +760,6 @@
   </si>
   <si>
     <t>Philosophy+theology centres for diocesan clergy - residences</t>
-  </si>
-  <si>
-    <t>Other visualization (other/world, snapshot)*</t>
   </si>
   <si>
     <t>Philosophy+theology centres for religious clergy - seminaries</t>
@@ -2312,9 +2273,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
-  <dimension ref="A1:Q91"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:D91"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2348,37 +2311,37 @@
         <v>56</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="H3" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="I3" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="J3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="K3" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="L3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2386,22 +2349,22 @@
         <v>57</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G4" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
@@ -2410,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -2431,7 +2394,7 @@
         <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2439,34 +2402,34 @@
         <v>58</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G5" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="H5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="I5" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="J5" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="K5" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2474,7 +2437,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>0</v>
@@ -2483,16 +2446,16 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H6" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2506,37 +2469,37 @@
         <v>59</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E8" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F8" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G8" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H8" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="I8" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="J8" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="K8" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="L8" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="M8" t="s">
         <v>10</v>
@@ -2550,114 +2513,114 @@
         <v>32</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F9" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E10" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G11" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H11" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="I11" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="J11" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="K11" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="L11" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="M11" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="E12" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F12" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G12" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H12" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="I12" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B13" s="31">
         <v>10</v>
@@ -2666,24 +2629,24 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="E13" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="F13" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G13" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="H13" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="B14" s="31">
         <v>11</v>
@@ -2692,30 +2655,30 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="E14" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="F14" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="G14" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="H14" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="I14" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="J14" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="B15" s="31">
         <v>12</v>
@@ -2724,21 +2687,21 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="E15" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="F15" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="G15" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B16" s="31">
         <v>13</v>
@@ -2767,7 +2730,7 @@
     </row>
     <row r="17" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="B17" s="31">
         <v>14</v>
@@ -2796,7 +2759,7 @@
     </row>
     <row r="18" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="B18" s="31">
         <v>15</v>
@@ -2825,7 +2788,7 @@
     </row>
     <row r="19" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="B19" s="31">
         <v>16</v>
@@ -2854,7 +2817,7 @@
     </row>
     <row r="20" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="B20" s="31">
         <v>17</v>
@@ -2883,7 +2846,7 @@
     </row>
     <row r="21" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B21" s="31">
         <v>18</v>
@@ -2912,7 +2875,7 @@
     </row>
     <row r="22" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="B22" s="31">
         <v>19</v>
@@ -2941,7 +2904,7 @@
     </row>
     <row r="23" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B23" s="31">
         <v>20</v>
@@ -2985,28 +2948,28 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E25" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="H25" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="I25" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3020,40 +2983,40 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="E26" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="F26" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="G26" t="s">
+        <v>267</v>
+      </c>
+      <c r="H26" t="s">
+        <v>270</v>
+      </c>
+      <c r="I26" t="s">
         <v>271</v>
       </c>
-      <c r="G26" t="s">
-        <v>280</v>
-      </c>
-      <c r="H26" t="s">
-        <v>283</v>
-      </c>
-      <c r="I26" t="s">
-        <v>284</v>
-      </c>
       <c r="J26" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="K26" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="L26" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="M26" s="26" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="N26" s="26" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3067,13 +3030,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="E27" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F27" t="s">
         <v>275</v>
-      </c>
-      <c r="F27" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3087,13 +3050,13 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="E28" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3110,33 +3073,33 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="H29" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="I29" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="J29" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="K29" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="L29" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="B30" s="32">
         <v>26</v>
@@ -3165,7 +3128,7 @@
     </row>
     <row r="31" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B31" s="32">
         <v>27</v>
@@ -3194,7 +3157,7 @@
     </row>
     <row r="32" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="B32" s="32">
         <v>28</v>
@@ -3223,7 +3186,7 @@
     </row>
     <row r="33" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="B33" s="32">
         <v>29</v>
@@ -3267,28 +3230,28 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="E35" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="F35" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="G35" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="H35" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="I35" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="J35" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="K35" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3302,21 +3265,21 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E36" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="F36" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="G36" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="B37" s="33">
         <v>32</v>
@@ -3325,40 +3288,40 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="E37" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="F37" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="G37" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="H37" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="I37" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="J37" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="K37" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="L37" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="M37" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="N37" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="O37" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3387,25 +3350,25 @@
         <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="H39" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="I39" t="s">
         <v>17</v>
       </c>
       <c r="J39" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="K39" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="L39" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="M39" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3416,227 +3379,227 @@
     </row>
     <row r="41" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="E41" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="F41" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G41" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="H41" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="I41" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="J41" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="K41" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="E42" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="F42" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="G42" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="H42" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="I42" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="J42" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="K42" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="E43" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="F43" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="G43" t="s">
+        <v>334</v>
+      </c>
+      <c r="H43" t="s">
+        <v>335</v>
+      </c>
+      <c r="I43" t="s">
+        <v>336</v>
+      </c>
+      <c r="J43" t="s">
+        <v>337</v>
+      </c>
+      <c r="K43" t="s">
         <v>347</v>
-      </c>
-      <c r="H43" t="s">
-        <v>348</v>
-      </c>
-      <c r="I43" t="s">
-        <v>349</v>
-      </c>
-      <c r="J43" t="s">
-        <v>350</v>
-      </c>
-      <c r="K43" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="E44" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="F44" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="G44" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="H44" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="I44" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="J44" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="K44" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E45" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="F45" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="E46" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="F46" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="E47" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="F47" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="E48" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="F48" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="B49" s="35">
         <v>36</v>
@@ -3645,36 +3608,36 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="E49" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="F49" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="G49" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="H49" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="I49" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="J49" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="K49" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="L49" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="B50" s="35">
         <v>37</v>
@@ -3683,30 +3646,30 @@
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="E50" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="F50" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="G50" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="H50" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="I50" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="J50" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="B51" s="35">
         <v>38</v>
@@ -3715,33 +3678,33 @@
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="E51" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="F51" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="G51" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="H51" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="I51" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="J51" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="K51" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="B52" s="35">
         <v>39</v>
@@ -3750,24 +3713,24 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="E52" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="F52" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="G52" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="H52" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="B53" s="35">
         <v>40</v>
@@ -3776,24 +3739,24 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="E53" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="F53" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="G53" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="H53" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="B54" s="35">
         <v>41</v>
@@ -3802,24 +3765,24 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="E54" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="F54" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="G54" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>18</v>
@@ -3845,10 +3808,10 @@
     </row>
     <row r="56" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>18</v>
@@ -3874,10 +3837,10 @@
     </row>
     <row r="57" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="B57" s="35" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>18</v>
@@ -3903,10 +3866,10 @@
     </row>
     <row r="58" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>18</v>
@@ -3932,10 +3895,10 @@
     </row>
     <row r="59" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>18</v>
@@ -3961,10 +3924,10 @@
     </row>
     <row r="60" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>18</v>
@@ -3990,10 +3953,10 @@
     </row>
     <row r="61" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>18</v>
@@ -4019,10 +3982,10 @@
     </row>
     <row r="62" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B62" s="35" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>18</v>
@@ -4048,10 +4011,10 @@
     </row>
     <row r="63" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="B63" s="35" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>18</v>
@@ -4077,10 +4040,10 @@
     </row>
     <row r="64" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>18</v>
@@ -4106,10 +4069,10 @@
     </row>
     <row r="65" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="B65" s="35" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>18</v>
@@ -4135,10 +4098,10 @@
     </row>
     <row r="66" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>18</v>
@@ -4164,10 +4127,10 @@
     </row>
     <row r="67" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="B67" s="35" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>18</v>
@@ -4193,10 +4156,10 @@
     </row>
     <row r="68" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="B68" s="35" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>18</v>
@@ -4222,10 +4185,10 @@
     </row>
     <row r="69" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="B69" s="35" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>18</v>
@@ -4251,10 +4214,10 @@
     </row>
     <row r="70" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="B70" s="35" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>18</v>
@@ -4280,10 +4243,10 @@
     </row>
     <row r="71" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="B71" s="35" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>27</v>
@@ -4309,10 +4272,10 @@
     </row>
     <row r="72" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="B72" s="35" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>29</v>
@@ -4338,10 +4301,10 @@
     </row>
     <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="B73" s="35" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>30</v>
@@ -4372,7 +4335,7 @@
     </row>
     <row r="75" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="B75" s="37">
         <v>51</v>
@@ -4381,33 +4344,33 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="E75" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="F75" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="G75" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="H75" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="I75" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="J75" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="K75" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="B76" s="37">
         <v>52</v>
@@ -4416,33 +4379,33 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="E76" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="F76" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="G76" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="H76" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="I76" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="J76" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="K76" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="B77" s="37">
         <v>53</v>
@@ -4451,28 +4414,28 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="E77" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="F77" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="G77" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="H77" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="I77" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="J77" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="K77" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4486,37 +4449,37 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
+        <v>409</v>
+      </c>
+      <c r="E78" t="s">
+        <v>410</v>
+      </c>
+      <c r="F78" t="s">
+        <v>411</v>
+      </c>
+      <c r="G78" t="s">
+        <v>412</v>
+      </c>
+      <c r="H78" t="s">
+        <v>424</v>
+      </c>
+      <c r="I78" t="s">
+        <v>423</v>
+      </c>
+      <c r="J78" t="s">
+        <v>419</v>
+      </c>
+      <c r="K78" t="s">
+        <v>420</v>
+      </c>
+      <c r="L78" t="s">
+        <v>421</v>
+      </c>
+      <c r="M78" t="s">
         <v>422</v>
       </c>
-      <c r="E78" t="s">
-        <v>423</v>
-      </c>
-      <c r="F78" t="s">
-        <v>424</v>
-      </c>
-      <c r="G78" t="s">
-        <v>425</v>
-      </c>
-      <c r="H78" t="s">
-        <v>437</v>
-      </c>
-      <c r="I78" t="s">
-        <v>436</v>
-      </c>
-      <c r="J78" t="s">
-        <v>432</v>
-      </c>
-      <c r="K78" t="s">
-        <v>433</v>
-      </c>
-      <c r="L78" t="s">
-        <v>434</v>
-      </c>
-      <c r="M78" t="s">
-        <v>435</v>
-      </c>
       <c r="N78" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4530,34 +4493,34 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E79" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="F79" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="G79" t="s">
+        <v>415</v>
+      </c>
+      <c r="H79" t="s">
+        <v>425</v>
+      </c>
+      <c r="I79" t="s">
         <v>428</v>
       </c>
-      <c r="H79" t="s">
-        <v>438</v>
-      </c>
-      <c r="I79" t="s">
-        <v>441</v>
-      </c>
       <c r="J79" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="K79" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="L79" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="M79" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4571,39 +4534,39 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="E80" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="F80" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="G80" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="H80" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="I80" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="J80" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="K80" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="L80" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="M80" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="B81" s="37">
         <v>57</v>
@@ -4612,27 +4575,27 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="E81" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="F81" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="G81" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="H81" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="I81" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B82" s="37">
         <v>58</v>
@@ -4641,21 +4604,21 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="E82" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="F82" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="G82" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="B83" s="37">
         <v>59</v>
@@ -4664,68 +4627,31 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="E83" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="F83" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="G83" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="H83" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="I83" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="J83" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="K83" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="L83" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>96</v>
-      </c>
-      <c r="C86" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>86</v>
-      </c>
-      <c r="C87" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>94</v>
-      </c>
-      <c r="C88" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>253</v>
-      </c>
-      <c r="C89" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>97</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -4742,10 +4668,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4786,16 +4712,16 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G3" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4803,7 +4729,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>67</v>
@@ -4832,7 +4758,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>73</v>
@@ -4861,7 +4787,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>66</v>
@@ -4890,7 +4816,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>66</v>
@@ -4945,7 +4871,7 @@
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>45</v>
@@ -4954,10 +4880,10 @@
         <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F9" t="s">
         <v>74</v>
@@ -4968,7 +4894,7 @@
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>46</v>
@@ -4977,16 +4903,16 @@
         <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="G10" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -5020,7 +4946,7 @@
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>49</v>
@@ -5029,36 +4955,36 @@
         <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="E12" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="G12" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="H12" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="I12" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="J12" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="K12" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>66</v>
@@ -5084,10 +5010,10 @@
     </row>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>66</v>
@@ -5113,10 +5039,10 @@
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>66</v>
@@ -5142,10 +5068,10 @@
     </row>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>66</v>
@@ -5171,7 +5097,7 @@
     </row>
     <row r="17" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>50</v>
@@ -5200,7 +5126,7 @@
     </row>
     <row r="18" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>51</v>
@@ -5229,7 +5155,7 @@
     </row>
     <row r="19" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>52</v>
@@ -5258,7 +5184,7 @@
     </row>
     <row r="20" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>53</v>
@@ -5293,7 +5219,7 @@
     </row>
     <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>75</v>
@@ -5302,21 +5228,21 @@
         <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="E22" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>66</v>
@@ -5342,10 +5268,10 @@
     </row>
     <row r="24" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>66</v>
@@ -5371,10 +5297,10 @@
     </row>
     <row r="25" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>66</v>
@@ -5400,10 +5326,10 @@
     </row>
     <row r="26" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>66</v>
@@ -5429,10 +5355,10 @@
     </row>
     <row r="27" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>66</v>
@@ -5458,10 +5384,10 @@
     </row>
     <row r="28" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>66</v>
@@ -5487,10 +5413,10 @@
     </row>
     <row r="29" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>66</v>
@@ -5516,10 +5442,10 @@
     </row>
     <row r="30" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>66</v>
@@ -5545,10 +5471,10 @@
     </row>
     <row r="31" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>66</v>
@@ -5574,10 +5500,10 @@
     </row>
     <row r="32" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>66</v>
@@ -5603,10 +5529,10 @@
     </row>
     <row r="33" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>66</v>
@@ -5632,10 +5558,10 @@
     </row>
     <row r="34" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>66</v>
@@ -5661,10 +5587,10 @@
     </row>
     <row r="35" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>66</v>
@@ -5690,10 +5616,10 @@
     </row>
     <row r="36" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>66</v>
@@ -5719,10 +5645,10 @@
     </row>
     <row r="37" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>66</v>
@@ -5748,10 +5674,10 @@
     </row>
     <row r="38" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>66</v>
@@ -5777,7 +5703,7 @@
     </row>
     <row r="39" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>76</v>
@@ -5786,21 +5712,21 @@
         <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="E39" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="F39" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="G39" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="B40" s="31" t="s">
         <v>77</v>
@@ -5809,16 +5735,16 @@
         <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="E40" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="F40" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="G40" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -5829,10 +5755,10 @@
     </row>
     <row r="42" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>66</v>
@@ -5858,10 +5784,10 @@
     </row>
     <row r="43" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="22" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>66</v>
@@ -5887,10 +5813,10 @@
     </row>
     <row r="44" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>66</v>
@@ -5916,10 +5842,10 @@
     </row>
     <row r="45" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>66</v>
@@ -5945,10 +5871,10 @@
     </row>
     <row r="46" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>66</v>
@@ -5974,10 +5900,10 @@
     </row>
     <row r="47" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>66</v>
@@ -6003,10 +5929,10 @@
     </row>
     <row r="48" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>66</v>
@@ -6032,10 +5958,10 @@
     </row>
     <row r="49" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>66</v>
@@ -6061,10 +5987,10 @@
     </row>
     <row r="50" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>66</v>
@@ -6090,10 +6016,10 @@
     </row>
     <row r="51" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>66</v>
@@ -6119,10 +6045,10 @@
     </row>
     <row r="52" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>66</v>
@@ -6148,10 +6074,10 @@
     </row>
     <row r="53" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>66</v>
@@ -6177,10 +6103,10 @@
     </row>
     <row r="54" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>66</v>
@@ -6206,10 +6132,10 @@
     </row>
     <row r="55" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>66</v>
@@ -6235,10 +6161,10 @@
     </row>
     <row r="56" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>66</v>
@@ -6264,10 +6190,10 @@
     </row>
     <row r="57" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="25" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>66</v>
@@ -6293,10 +6219,10 @@
     </row>
     <row r="58" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="25" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>66</v>
@@ -6322,10 +6248,10 @@
     </row>
     <row r="59" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="25" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>66</v>
@@ -6351,10 +6277,10 @@
     </row>
     <row r="60" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>66</v>
@@ -6380,10 +6306,10 @@
     </row>
     <row r="61" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>66</v>
@@ -6409,10 +6335,10 @@
     </row>
     <row r="62" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>66</v>
@@ -6438,10 +6364,10 @@
     </row>
     <row r="63" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>66</v>
@@ -6467,10 +6393,10 @@
     </row>
     <row r="64" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>66</v>
@@ -6496,10 +6422,10 @@
     </row>
     <row r="65" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>66</v>
@@ -6525,10 +6451,10 @@
     </row>
     <row r="66" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>66</v>
@@ -6554,7 +6480,7 @@
     </row>
     <row r="67" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="B67" s="32" t="s">
         <v>79</v>
@@ -6583,7 +6509,7 @@
     </row>
     <row r="68" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="27" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="B68" s="32" t="s">
         <v>80</v>
@@ -6612,7 +6538,7 @@
     </row>
     <row r="69" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="B69" s="32" t="s">
         <v>81</v>
@@ -6653,19 +6579,19 @@
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="F70" t="s">
         <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="H70" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="I70" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -6676,7 +6602,7 @@
     </row>
     <row r="72" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="B72" s="33" t="s">
         <v>84</v>
@@ -6705,7 +6631,7 @@
     </row>
     <row r="73" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="B73" s="33" t="s">
         <v>83</v>
@@ -6757,46 +6683,9 @@
       <c r="A78" s="11"/>
       <c r="B78" s="37"/>
     </row>
-    <row r="79" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>96</v>
-      </c>
-      <c r="C79" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>86</v>
-      </c>
-      <c r="C80" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>253</v>
-      </c>
-      <c r="C82" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11"/>
       <c r="B83" s="37"/>
-    </row>
-    <row r="84" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>97</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>

</xml_diff>

<commit_message>
changed some names (for real)
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8DD64F-A47D-4F0A-B93C-9BDFDCBC02D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E81782-96F6-4814-A9C1-9742C13B0840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -2266,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4661,7 +4661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added split tables 32-1 and 32-2
splitting needed to separate two distinct variables in a time series table
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E81782-96F6-4814-A9C1-9742C13B0840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CBBF12-4AAB-4F47-983E-236372F6211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="533">
   <si>
     <t>Countries</t>
   </si>
@@ -900,45 +900,6 @@
     <t>First Communions per 1000 Catholics</t>
   </si>
   <si>
-    <t>Infant baptisms (people up to 7 years old) per 1000 Catholics - 2017</t>
-  </si>
-  <si>
-    <t>Infant baptisms (people up to 7 years old) per 1000 Catholics - 2018</t>
-  </si>
-  <si>
-    <t>Infant baptisms (people up to 7 years old) per 1000 Catholics - 2019</t>
-  </si>
-  <si>
-    <t>Infant baptisms (people up to 7 years old) per 1000 Catholics - 2020</t>
-  </si>
-  <si>
-    <t>Infant baptisms (people up to 7 years old) per 1000 Catholics - 2021</t>
-  </si>
-  <si>
-    <t>Infant baptisms (people up to 7 years old) per 1000 Catholics - 2022</t>
-  </si>
-  <si>
-    <t>Marriages per 1000 Catholics - 2017</t>
-  </si>
-  <si>
-    <t>Marriages per 1000 Catholics - 2018</t>
-  </si>
-  <si>
-    <t>Marriages per 1000 Catholics - 2019</t>
-  </si>
-  <si>
-    <t>Marriages per 1000 Catholics - 2020</t>
-  </si>
-  <si>
-    <t>Marriages per 1000 Catholics - 2021</t>
-  </si>
-  <si>
-    <t>Marriages per 1000 Catholics - 2022</t>
-  </si>
-  <si>
-    <t>Infant baptisms (people up to 7 years old) and marriages per 1000 Catholics</t>
-  </si>
-  <si>
     <t>Homes for old, chronically ill, and disabled people</t>
   </si>
   <si>
@@ -1669,6 +1630,12 @@
   </si>
   <si>
     <t>Bishops</t>
+  </si>
+  <si>
+    <t>32-2</t>
+  </si>
+  <si>
+    <t>32-1</t>
   </si>
 </sst>
 </file>
@@ -2264,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2302,7 +2269,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>0</v>
@@ -2329,7 +2296,7 @@
         <v>170</v>
       </c>
       <c r="K3" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="L3" t="s">
         <v>183</v>
@@ -2340,7 +2307,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>0</v>
@@ -2364,7 +2331,7 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -2393,7 +2360,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>0</v>
@@ -2428,7 +2395,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>0</v>
@@ -2460,7 +2427,7 @@
         <v>55</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>0</v>
@@ -2469,7 +2436,7 @@
         <v>185</v>
       </c>
       <c r="E8" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="F8" t="s">
         <v>186</v>
@@ -2487,10 +2454,10 @@
         <v>215</v>
       </c>
       <c r="K8" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="L8" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="M8" t="s">
         <v>10</v>
@@ -2504,7 +2471,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>0</v>
@@ -2516,7 +2483,7 @@
         <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2524,7 +2491,7 @@
         <v>191</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>0</v>
@@ -2544,7 +2511,7 @@
         <v>193</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>0</v>
@@ -2585,7 +2552,7 @@
         <v>204</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
@@ -2620,16 +2587,16 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="E13" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="F13" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="G13" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="H13" t="s">
         <v>208</v>
@@ -2637,7 +2604,7 @@
     </row>
     <row r="14" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="B14" s="31">
         <v>11</v>
@@ -2649,27 +2616,27 @@
         <v>209</v>
       </c>
       <c r="E14" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="F14" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="G14" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="H14" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="I14" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="J14" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="B15" s="31">
         <v>12</v>
@@ -2678,16 +2645,16 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="E15" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="F15" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="G15" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2721,7 +2688,7 @@
     </row>
     <row r="17" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="B17" s="31">
         <v>14</v>
@@ -2750,7 +2717,7 @@
     </row>
     <row r="18" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="B18" s="31">
         <v>15</v>
@@ -2779,7 +2746,7 @@
     </row>
     <row r="19" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="B19" s="31">
         <v>16</v>
@@ -2808,7 +2775,7 @@
     </row>
     <row r="20" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="B20" s="31">
         <v>17</v>
@@ -3175,7 +3142,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>253</v>
       </c>
@@ -3204,13 +3171,13 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="32"/>
     </row>
-    <row r="35" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
         <v>36</v>
       </c>
@@ -3245,7 +3212,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>37</v>
       </c>
@@ -3268,541 +3235,523 @@
         <v>286</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="B37" s="33">
-        <v>32</v>
+        <v>281</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>532</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37">
+        <v>2017</v>
+      </c>
+      <c r="E37">
+        <v>2018</v>
+      </c>
+      <c r="F37">
+        <v>2019</v>
+      </c>
+      <c r="G37">
+        <v>2020</v>
+      </c>
+      <c r="H37">
+        <v>2021</v>
+      </c>
+      <c r="I37">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>531</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>2017</v>
+      </c>
+      <c r="E38">
+        <v>2018</v>
+      </c>
+      <c r="F38">
+        <v>2019</v>
+      </c>
+      <c r="G38">
+        <v>2020</v>
+      </c>
+      <c r="H38">
+        <v>2021</v>
+      </c>
+      <c r="I38">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="33"/>
+    </row>
+    <row r="40" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="34">
+        <v>33</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" t="s">
         <v>287</v>
       </c>
-      <c r="E37" t="s">
+      <c r="H40" t="s">
         <v>288</v>
       </c>
-      <c r="F37" t="s">
+      <c r="I40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" t="s">
         <v>289</v>
       </c>
-      <c r="G37" t="s">
+      <c r="K40" t="s">
         <v>290</v>
       </c>
-      <c r="H37" t="s">
+      <c r="L40" t="s">
+        <v>298</v>
+      </c>
+      <c r="M40" t="s">
         <v>291</v>
       </c>
-      <c r="I37" t="s">
-        <v>292</v>
-      </c>
-      <c r="J37" t="s">
-        <v>293</v>
-      </c>
-      <c r="K37" t="s">
-        <v>294</v>
-      </c>
-      <c r="L37" t="s">
-        <v>295</v>
-      </c>
-      <c r="M37" t="s">
-        <v>296</v>
-      </c>
-      <c r="N37" t="s">
-        <v>297</v>
-      </c>
-      <c r="O37" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="33"/>
-    </row>
-    <row r="39" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="34">
-        <v>33</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" t="s">
-        <v>300</v>
-      </c>
-      <c r="H39" t="s">
-        <v>301</v>
-      </c>
-      <c r="I39" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" t="s">
-        <v>302</v>
-      </c>
-      <c r="K39" t="s">
-        <v>303</v>
-      </c>
-      <c r="L39" t="s">
-        <v>311</v>
-      </c>
-      <c r="M39" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+    </row>
+    <row r="41" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="34"/>
-    </row>
-    <row r="41" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="34"/>
+    </row>
+    <row r="42" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B42" s="35" t="s">
         <v>129</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" t="s">
-        <v>472</v>
-      </c>
-      <c r="E41" t="s">
-        <v>469</v>
-      </c>
-      <c r="F41" t="s">
-        <v>312</v>
-      </c>
-      <c r="G41" t="s">
-        <v>313</v>
-      </c>
-      <c r="H41" t="s">
-        <v>314</v>
-      </c>
-      <c r="I41" t="s">
-        <v>315</v>
-      </c>
-      <c r="J41" t="s">
-        <v>316</v>
-      </c>
-      <c r="K41" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>130</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="E42" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="F42" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="G42" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="H42" t="s">
+        <v>301</v>
+      </c>
+      <c r="I42" t="s">
+        <v>302</v>
+      </c>
+      <c r="J42" t="s">
+        <v>303</v>
+      </c>
+      <c r="K42" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="I42" t="s">
-        <v>320</v>
-      </c>
-      <c r="J42" t="s">
-        <v>321</v>
-      </c>
-      <c r="K42" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
-        <v>333</v>
-      </c>
       <c r="B43" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="E43" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="F43" t="s">
+        <v>304</v>
+      </c>
+      <c r="G43" t="s">
+        <v>305</v>
+      </c>
+      <c r="H43" t="s">
+        <v>306</v>
+      </c>
+      <c r="I43" t="s">
+        <v>307</v>
+      </c>
+      <c r="J43" t="s">
+        <v>308</v>
+      </c>
+      <c r="K43" t="s">
         <v>322</v>
       </c>
-      <c r="G43" t="s">
-        <v>323</v>
-      </c>
-      <c r="H43" t="s">
-        <v>324</v>
-      </c>
-      <c r="I43" t="s">
-        <v>325</v>
-      </c>
-      <c r="J43" t="s">
-        <v>326</v>
-      </c>
-      <c r="K43" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="E44" t="s">
-        <v>363</v>
+        <v>458</v>
       </c>
       <c r="F44" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="G44" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="H44" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="I44" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="J44" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="K44" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>354</v>
+        <v>462</v>
       </c>
       <c r="E45" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F45" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+      <c r="G45" t="s">
+        <v>315</v>
+      </c>
+      <c r="H45" t="s">
+        <v>316</v>
+      </c>
+      <c r="I45" t="s">
+        <v>317</v>
+      </c>
+      <c r="J45" t="s">
+        <v>318</v>
+      </c>
+      <c r="K45" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>476</v>
+        <v>341</v>
       </c>
       <c r="E46" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F46" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>345</v>
+        <v>463</v>
       </c>
       <c r="E47" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="F47" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="E48" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="F48" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>358</v>
-      </c>
-      <c r="B49" s="35">
-        <v>36</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>0</v>
+        <v>327</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>469</v>
+        <v>333</v>
       </c>
       <c r="E49" t="s">
-        <v>312</v>
+        <v>336</v>
       </c>
       <c r="F49" t="s">
-        <v>313</v>
-      </c>
-      <c r="G49" t="s">
-        <v>314</v>
-      </c>
-      <c r="H49" t="s">
-        <v>315</v>
-      </c>
-      <c r="I49" t="s">
-        <v>316</v>
-      </c>
-      <c r="J49" t="s">
-        <v>354</v>
-      </c>
-      <c r="K49" t="s">
-        <v>355</v>
-      </c>
-      <c r="L49" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B50" s="35">
-        <v>37</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>356</v>
+        <v>456</v>
       </c>
       <c r="E50" t="s">
-        <v>518</v>
+        <v>299</v>
       </c>
       <c r="F50" t="s">
-        <v>511</v>
+        <v>300</v>
       </c>
       <c r="G50" t="s">
-        <v>507</v>
+        <v>301</v>
       </c>
       <c r="H50" t="s">
-        <v>478</v>
+        <v>302</v>
       </c>
       <c r="I50" t="s">
-        <v>479</v>
+        <v>303</v>
       </c>
       <c r="J50" t="s">
-        <v>483</v>
+        <v>341</v>
+      </c>
+      <c r="K50" t="s">
+        <v>342</v>
+      </c>
+      <c r="L50" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="B51" s="35">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="E51" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
       <c r="F51" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="G51" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
       <c r="H51" t="s">
-        <v>512</v>
+        <v>465</v>
       </c>
       <c r="I51" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="J51" t="s">
-        <v>481</v>
-      </c>
-      <c r="K51" t="s">
-        <v>316</v>
+        <v>470</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B52" s="35">
-        <v>39</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>484</v>
+        <v>344</v>
       </c>
       <c r="E52" t="s">
-        <v>487</v>
+        <v>509</v>
       </c>
       <c r="F52" t="s">
-        <v>488</v>
+        <v>506</v>
       </c>
       <c r="G52" t="s">
-        <v>489</v>
+        <v>510</v>
       </c>
       <c r="H52" t="s">
-        <v>490</v>
+        <v>499</v>
+      </c>
+      <c r="I52" t="s">
+        <v>467</v>
+      </c>
+      <c r="J52" t="s">
+        <v>468</v>
+      </c>
+      <c r="K52" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B53" s="35">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="E53" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="F53" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="G53" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="H53" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="B54" s="35">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E54" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
       <c r="F54" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="G54" t="s">
-        <v>497</v>
+        <v>480</v>
+      </c>
+      <c r="H54" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="B55" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55">
-        <v>2017</v>
-      </c>
-      <c r="E55">
-        <v>2018</v>
-      </c>
-      <c r="F55">
-        <v>2019</v>
-      </c>
-      <c r="G55">
-        <v>2020</v>
-      </c>
-      <c r="H55">
-        <v>2021</v>
-      </c>
-      <c r="I55">
-        <v>2022</v>
+        <v>351</v>
+      </c>
+      <c r="B55" s="35">
+        <v>41</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>473</v>
+      </c>
+      <c r="E55" t="s">
+        <v>482</v>
+      </c>
+      <c r="F55" t="s">
+        <v>483</v>
+      </c>
+      <c r="G55" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>18</v>
@@ -3828,10 +3777,10 @@
     </row>
     <row r="57" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>520</v>
+        <v>297</v>
       </c>
       <c r="B57" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>18</v>
@@ -3857,10 +3806,10 @@
     </row>
     <row r="58" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>18</v>
@@ -3889,7 +3838,7 @@
         <v>508</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>18</v>
@@ -3915,10 +3864,10 @@
     </row>
     <row r="60" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>18</v>
@@ -3944,10 +3893,10 @@
     </row>
     <row r="61" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>18</v>
@@ -3973,10 +3922,10 @@
     </row>
     <row r="62" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="B62" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>18</v>
@@ -4002,10 +3951,10 @@
     </row>
     <row r="63" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>365</v>
+        <v>501</v>
       </c>
       <c r="B63" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>18</v>
@@ -4031,10 +3980,10 @@
     </row>
     <row r="64" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>18</v>
@@ -4060,10 +4009,10 @@
     </row>
     <row r="65" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B65" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>18</v>
@@ -4089,10 +4038,10 @@
     </row>
     <row r="66" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>18</v>
@@ -4118,10 +4067,10 @@
     </row>
     <row r="67" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="B67" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>18</v>
@@ -4147,10 +4096,10 @@
     </row>
     <row r="68" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B68" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>18</v>
@@ -4176,10 +4125,10 @@
     </row>
     <row r="69" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="B69" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>18</v>
@@ -4205,10 +4154,10 @@
     </row>
     <row r="70" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B70" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>18</v>
@@ -4234,13 +4183,13 @@
     </row>
     <row r="71" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="B71" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D71">
         <v>2017</v>
@@ -4263,13 +4212,13 @@
     </row>
     <row r="72" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B72" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D72">
         <v>2017</v>
@@ -4292,363 +4241,392 @@
     </row>
     <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B73" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73">
+        <v>2017</v>
+      </c>
+      <c r="E73">
+        <v>2018</v>
+      </c>
+      <c r="F73">
+        <v>2019</v>
+      </c>
+      <c r="G73">
+        <v>2020</v>
+      </c>
+      <c r="H73">
+        <v>2021</v>
+      </c>
+      <c r="I73">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="B74" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C74" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D73">
-        <v>2017</v>
-      </c>
-      <c r="E73">
-        <v>2018</v>
-      </c>
-      <c r="F73">
-        <v>2019</v>
-      </c>
-      <c r="G73">
-        <v>2020</v>
-      </c>
-      <c r="H73">
-        <v>2021</v>
-      </c>
-      <c r="I73">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
+      <c r="D74">
+        <v>2017</v>
+      </c>
+      <c r="E74">
+        <v>2018</v>
+      </c>
+      <c r="F74">
+        <v>2019</v>
+      </c>
+      <c r="G74">
+        <v>2020</v>
+      </c>
+      <c r="H74">
+        <v>2021</v>
+      </c>
+      <c r="I74">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="B75" s="37">
-        <v>51</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" t="s">
-        <v>374</v>
-      </c>
-      <c r="E75" t="s">
-        <v>375</v>
-      </c>
-      <c r="F75" t="s">
-        <v>376</v>
-      </c>
-      <c r="G75" t="s">
-        <v>377</v>
-      </c>
-      <c r="H75" t="s">
-        <v>378</v>
-      </c>
-      <c r="I75" t="s">
-        <v>379</v>
-      </c>
-      <c r="J75" t="s">
-        <v>380</v>
-      </c>
-      <c r="K75" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="B76" s="37">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="E76" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="F76" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="G76" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="H76" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="I76" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="J76" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="K76" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="B77" s="37">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="E77" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
       <c r="F77" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="G77" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="H77" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="I77" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="J77" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="K77" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>38</v>
+        <v>437</v>
       </c>
       <c r="B78" s="37">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="E78" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="F78" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="G78" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="H78" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="I78" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
       <c r="J78" t="s">
-        <v>408</v>
+        <v>383</v>
       </c>
       <c r="K78" t="s">
-        <v>409</v>
-      </c>
-      <c r="L78" t="s">
-        <v>410</v>
-      </c>
-      <c r="M78" t="s">
-        <v>411</v>
-      </c>
-      <c r="N78" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B79" s="37">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D79" t="s">
+        <v>385</v>
+      </c>
+      <c r="E79" t="s">
+        <v>386</v>
+      </c>
+      <c r="F79" t="s">
+        <v>387</v>
+      </c>
+      <c r="G79" t="s">
+        <v>388</v>
+      </c>
+      <c r="H79" t="s">
+        <v>400</v>
+      </c>
+      <c r="I79" t="s">
+        <v>399</v>
+      </c>
+      <c r="J79" t="s">
+        <v>395</v>
+      </c>
+      <c r="K79" t="s">
+        <v>396</v>
+      </c>
+      <c r="L79" t="s">
+        <v>397</v>
+      </c>
+      <c r="M79" t="s">
+        <v>398</v>
+      </c>
+      <c r="N79" t="s">
         <v>402</v>
-      </c>
-      <c r="E79" t="s">
-        <v>416</v>
-      </c>
-      <c r="F79" t="s">
-        <v>403</v>
-      </c>
-      <c r="G79" t="s">
-        <v>404</v>
-      </c>
-      <c r="H79" t="s">
-        <v>414</v>
-      </c>
-      <c r="I79" t="s">
-        <v>417</v>
-      </c>
-      <c r="J79" t="s">
-        <v>418</v>
-      </c>
-      <c r="K79" t="s">
-        <v>419</v>
-      </c>
-      <c r="L79" t="s">
-        <v>420</v>
-      </c>
-      <c r="M79" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B80" s="37">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D80" t="s">
+        <v>389</v>
+      </c>
+      <c r="E80" t="s">
+        <v>403</v>
+      </c>
+      <c r="F80" t="s">
+        <v>390</v>
+      </c>
+      <c r="G80" t="s">
+        <v>391</v>
+      </c>
+      <c r="H80" t="s">
+        <v>401</v>
+      </c>
+      <c r="I80" t="s">
+        <v>404</v>
+      </c>
+      <c r="J80" t="s">
         <v>405</v>
       </c>
-      <c r="E80" t="s">
-        <v>422</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="K80" t="s">
         <v>406</v>
       </c>
-      <c r="G80" t="s">
+      <c r="L80" t="s">
         <v>407</v>
       </c>
-      <c r="H80" t="s">
-        <v>423</v>
-      </c>
-      <c r="I80" t="s">
-        <v>424</v>
-      </c>
-      <c r="J80" t="s">
-        <v>425</v>
-      </c>
-      <c r="K80" t="s">
-        <v>426</v>
-      </c>
-      <c r="L80" t="s">
-        <v>427</v>
-      </c>
       <c r="M80" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
-        <v>451</v>
+        <v>40</v>
       </c>
       <c r="B81" s="37">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>429</v>
+        <v>392</v>
       </c>
       <c r="E81" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="F81" t="s">
-        <v>431</v>
+        <v>393</v>
       </c>
       <c r="G81" t="s">
-        <v>432</v>
+        <v>394</v>
       </c>
       <c r="H81" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="I81" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+      <c r="J81" t="s">
+        <v>412</v>
+      </c>
+      <c r="K81" t="s">
+        <v>413</v>
+      </c>
+      <c r="L81" t="s">
+        <v>414</v>
+      </c>
+      <c r="M81" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="B82" s="37">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
       <c r="E82" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="F82" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="G82" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+      <c r="H82" t="s">
+        <v>420</v>
+      </c>
+      <c r="I82" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="B83" s="37">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="E83" t="s">
+        <v>423</v>
+      </c>
+      <c r="F83" t="s">
+        <v>424</v>
+      </c>
+      <c r="G83" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
         <v>440</v>
       </c>
-      <c r="F83" t="s">
-        <v>441</v>
-      </c>
-      <c r="G83" t="s">
-        <v>442</v>
-      </c>
-      <c r="H83" t="s">
-        <v>443</v>
-      </c>
-      <c r="I83" t="s">
-        <v>444</v>
-      </c>
-      <c r="J83" t="s">
-        <v>446</v>
-      </c>
-      <c r="K83" t="s">
-        <v>447</v>
-      </c>
-      <c r="L83" t="s">
-        <v>445</v>
+      <c r="B84" s="37">
+        <v>59</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>426</v>
+      </c>
+      <c r="E84" t="s">
+        <v>427</v>
+      </c>
+      <c r="F84" t="s">
+        <v>428</v>
+      </c>
+      <c r="G84" t="s">
+        <v>429</v>
+      </c>
+      <c r="H84" t="s">
+        <v>430</v>
+      </c>
+      <c r="I84" t="s">
+        <v>431</v>
+      </c>
+      <c r="J84" t="s">
+        <v>433</v>
+      </c>
+      <c r="K84" t="s">
+        <v>434</v>
+      </c>
+      <c r="L84" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
-  <conditionalFormatting sqref="A2:XFD83">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="A2:XFD84">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -4661,8 +4639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4694,7 +4672,7 @@
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>41</v>
@@ -4717,7 +4695,7 @@
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>80</v>
@@ -4746,7 +4724,7 @@
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>81</v>
@@ -4804,7 +4782,7 @@
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>83</v>
@@ -4862,7 +4840,7 @@
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>44</v>
@@ -4885,7 +4863,7 @@
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>45</v>
@@ -4937,7 +4915,7 @@
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>47</v>
@@ -4958,10 +4936,10 @@
         <v>159</v>
       </c>
       <c r="H12" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="I12" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="J12" t="s">
         <v>183</v>
@@ -5001,7 +4979,7 @@
     </row>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>85</v>
@@ -5059,7 +5037,7 @@
     </row>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>87</v>
@@ -5210,7 +5188,7 @@
     </row>
     <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>69</v>
@@ -5219,10 +5197,10 @@
         <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="E22" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="F22" t="s">
         <v>185</v>
@@ -5230,7 +5208,7 @@
     </row>
     <row r="23" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>88</v>
@@ -5259,7 +5237,7 @@
     </row>
     <row r="24" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>89</v>
@@ -5346,7 +5324,7 @@
     </row>
     <row r="27" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>92</v>
@@ -5375,7 +5353,7 @@
     </row>
     <row r="28" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>93</v>
@@ -5404,7 +5382,7 @@
     </row>
     <row r="29" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>94</v>
@@ -5433,7 +5411,7 @@
     </row>
     <row r="30" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>95</v>
@@ -5491,7 +5469,7 @@
     </row>
     <row r="32" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>97</v>
@@ -5607,7 +5585,7 @@
     </row>
     <row r="36" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>101</v>
@@ -5694,7 +5672,7 @@
     </row>
     <row r="39" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>70</v>
@@ -5703,21 +5681,21 @@
         <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="E39" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="F39" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="G39" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="B40" s="31" t="s">
         <v>71</v>
@@ -5726,16 +5704,16 @@
         <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="E40" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="F40" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="G40" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -6471,7 +6449,7 @@
     </row>
     <row r="67" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="B67" s="32" t="s">
         <v>73</v>
@@ -6681,7 +6659,7 @@
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="A2:XFD73">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
corrections in sheet 2
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37B2813-1E48-46E3-BF53-92B98C288D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032E5F8-E52F-4387-B5C5-40C470EAECEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="537">
   <si>
     <t>Countries</t>
   </si>
@@ -1636,6 +1636,18 @@
   </si>
   <si>
     <t>32-1</t>
+  </si>
+  <si>
+    <t>Secondary schools and philosophy+theology centres for diocesan clergy - seminaries</t>
+  </si>
+  <si>
+    <t>Secondary schools and philosophy+theology centres for diocesan clergy - residences</t>
+  </si>
+  <si>
+    <t>Secondary schools and philosophy+theology centres for religious clergy - seminaries</t>
+  </si>
+  <si>
+    <t>Secondary schools and philosophy+theology centres for religious clergy - residences</t>
   </si>
 </sst>
 </file>
@@ -2233,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3075,7 +3087,7 @@
         <v>2019</v>
       </c>
       <c r="G30" s="28">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="H30">
         <v>2021</v>
@@ -4639,8 +4651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5985,7 +5997,7 @@
     </row>
     <row r="51" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
-        <v>228</v>
+        <v>533</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>113</v>
@@ -6014,7 +6026,7 @@
     </row>
     <row r="52" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
-        <v>229</v>
+        <v>534</v>
       </c>
       <c r="B52" s="32" t="s">
         <v>114</v>
@@ -6043,7 +6055,7 @@
     </row>
     <row r="53" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
-        <v>230</v>
+        <v>535</v>
       </c>
       <c r="B53" s="32" t="s">
         <v>115</v>
@@ -6072,7 +6084,7 @@
     </row>
     <row r="54" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>231</v>
+        <v>536</v>
       </c>
       <c r="B54" s="32" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
corrected table 38 names
</commit_message>
<xml_diff>
--- a/data overview.xlsx
+++ b/data overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032E5F8-E52F-4387-B5C5-40C470EAECEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD5FF16-639D-457A-A54D-441ACE8DA900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD2F443-CD9A-43A3-B3DC-4A8FDC20553E}"/>
   </bookViews>
   <sheets>
     <sheet name="analytical tables (Arabic#)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="538">
   <si>
     <t>Countries</t>
   </si>
@@ -1071,9 +1071,6 @@
     <t>Priests in ISPRs for men on January 1</t>
   </si>
   <si>
-    <t>Non-priest religious men in ISPRs on January 1</t>
-  </si>
-  <si>
     <t>ISPRs for men. Houses and members on 31 December 2022</t>
   </si>
   <si>
@@ -1440,12 +1437,6 @@
     <t xml:space="preserve">Yearly variation in number of priests in ISPRs for men (overall balance) </t>
   </si>
   <si>
-    <t xml:space="preserve">Yearly variation in number of non-priest religious men in ISPRs for other reasons </t>
-  </si>
-  <si>
-    <t>Yearly variation in number of non-priest religious men in ISPRs (overall balance)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yearly variation in number of diocesan priests for other reasons </t>
   </si>
   <si>
@@ -1536,9 +1527,6 @@
     <t>Yearly deaths of priests in ISPRs for men</t>
   </si>
   <si>
-    <t>Yearly deaths of non-priest religious men in ISPRs</t>
-  </si>
-  <si>
     <t>Yearly deaths of religious priests in ISPRs</t>
   </si>
   <si>
@@ -1557,21 +1545,12 @@
     <t>Yearly ordinations of priests in ISPRs for men</t>
   </si>
   <si>
-    <t>Yearly ordinations of non-priest religious men in ISPRs</t>
-  </si>
-  <si>
     <t>Yearly ordinations of religious priests in ISPRs</t>
   </si>
   <si>
     <t>Yearly ordinations of religious priests ISPRs - index numbers (base 2013 = 100)</t>
   </si>
   <si>
-    <t>Yearly professions of non-priest religious men in ISPRs</t>
-  </si>
-  <si>
-    <t>Yearly departures of non-priest religious men in ISPRs</t>
-  </si>
-  <si>
     <t>Other pastoral centres</t>
   </si>
   <si>
@@ -1648,6 +1627,30 @@
   </si>
   <si>
     <t>Secondary schools and philosophy+theology centres for religious clergy - residences</t>
+  </si>
+  <si>
+    <t>Non-priest religious members and seminarians in ISPRs for men</t>
+  </si>
+  <si>
+    <t>Yearly variation in number of non-priest religious men and seminarians in ISPRs (overall balance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yearly variation in number of non-priest religious men and seminarians in ISPRs for other reasons </t>
+  </si>
+  <si>
+    <t>Yearly deaths of non-priest religious men and seminarians in ISPRs</t>
+  </si>
+  <si>
+    <t>Yearly departures of non-priest religious men and seminarians in ISPRs</t>
+  </si>
+  <si>
+    <t>Yearly ordinations of non-priest religious men and seminarians in ISPRs</t>
+  </si>
+  <si>
+    <t>Yearly professions of non-priest religious men and seminarians in ISPRs</t>
+  </si>
+  <si>
+    <t>Non-priest religious men and seminarians in ISPRs on January 1</t>
   </si>
 </sst>
 </file>
@@ -2245,8 +2248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD27EDBA-F404-4196-A455-7B46C4A9E8FA}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="E38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2281,7 +2284,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>0</v>
@@ -2308,7 +2311,7 @@
         <v>170</v>
       </c>
       <c r="K3" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="L3" t="s">
         <v>183</v>
@@ -2319,7 +2322,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>0</v>
@@ -2372,7 +2375,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>0</v>
@@ -2407,7 +2410,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>0</v>
@@ -2439,7 +2442,7 @@
         <v>55</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>0</v>
@@ -2448,7 +2451,7 @@
         <v>185</v>
       </c>
       <c r="E8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F8" t="s">
         <v>186</v>
@@ -2483,7 +2486,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>0</v>
@@ -2503,7 +2506,7 @@
         <v>191</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>0</v>
@@ -2523,7 +2526,7 @@
         <v>193</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>0</v>
@@ -2564,7 +2567,7 @@
         <v>204</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
@@ -2599,16 +2602,16 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
+        <v>447</v>
+      </c>
+      <c r="E13" t="s">
         <v>448</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>440</v>
+      </c>
+      <c r="G13" t="s">
         <v>449</v>
-      </c>
-      <c r="F13" t="s">
-        <v>441</v>
-      </c>
-      <c r="G13" t="s">
-        <v>450</v>
       </c>
       <c r="H13" t="s">
         <v>208</v>
@@ -2616,7 +2619,7 @@
     </row>
     <row r="14" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B14" s="31">
         <v>11</v>
@@ -2628,27 +2631,27 @@
         <v>209</v>
       </c>
       <c r="E14" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="G14" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="H14" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B15" s="31">
         <v>12</v>
@@ -2657,16 +2660,16 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
+        <v>482</v>
+      </c>
+      <c r="E15" t="s">
         <v>485</v>
       </c>
-      <c r="E15" t="s">
-        <v>488</v>
-      </c>
       <c r="F15" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="G15" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2700,7 +2703,7 @@
     </row>
     <row r="17" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B17" s="31">
         <v>14</v>
@@ -2729,7 +2732,7 @@
     </row>
     <row r="18" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B18" s="31">
         <v>15</v>
@@ -2758,7 +2761,7 @@
     </row>
     <row r="19" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B19" s="31">
         <v>16</v>
@@ -2787,7 +2790,7 @@
     </row>
     <row r="20" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B20" s="31">
         <v>17</v>
@@ -3252,7 +3255,7 @@
         <v>281</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>0</v>
@@ -3281,7 +3284,7 @@
         <v>282</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>0</v>
@@ -3369,10 +3372,10 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E42" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F42" t="s">
         <v>299</v>
@@ -3390,7 +3393,7 @@
         <v>303</v>
       </c>
       <c r="K42" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3404,10 +3407,10 @@
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E43" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F43" t="s">
         <v>304</v>
@@ -3439,10 +3442,10 @@
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E44" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F44" t="s">
         <v>309</v>
@@ -3474,10 +3477,10 @@
         <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E45" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F45" t="s">
         <v>314</v>
@@ -3515,7 +3518,7 @@
         <v>342</v>
       </c>
       <c r="F46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3529,7 +3532,7 @@
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E47" t="s">
         <v>334</v>
@@ -3580,7 +3583,7 @@
     </row>
     <row r="50" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B50" s="35">
         <v>36</v>
@@ -3589,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E50" t="s">
         <v>299</v>
@@ -3618,7 +3621,7 @@
     </row>
     <row r="51" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B51" s="35">
         <v>37</v>
@@ -3630,27 +3633,27 @@
         <v>343</v>
       </c>
       <c r="E51" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F51" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="G51" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H51" t="s">
+        <v>464</v>
+      </c>
+      <c r="I51" t="s">
         <v>465</v>
       </c>
-      <c r="I51" t="s">
-        <v>466</v>
-      </c>
       <c r="J51" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B52" s="35">
         <v>38</v>
@@ -3659,33 +3662,33 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>344</v>
+        <v>537</v>
       </c>
       <c r="E52" t="s">
-        <v>509</v>
+        <v>536</v>
       </c>
       <c r="F52" t="s">
-        <v>506</v>
+        <v>535</v>
       </c>
       <c r="G52" t="s">
-        <v>510</v>
+        <v>534</v>
       </c>
       <c r="H52" t="s">
-        <v>499</v>
+        <v>533</v>
       </c>
       <c r="I52" t="s">
-        <v>467</v>
+        <v>532</v>
       </c>
       <c r="J52" t="s">
-        <v>468</v>
+        <v>531</v>
       </c>
       <c r="K52" t="s">
-        <v>303</v>
+        <v>530</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B53" s="35">
         <v>39</v>
@@ -3694,24 +3697,24 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
+        <v>468</v>
+      </c>
+      <c r="E53" t="s">
         <v>471</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
+        <v>472</v>
+      </c>
+      <c r="G53" t="s">
+        <v>473</v>
+      </c>
+      <c r="H53" t="s">
         <v>474</v>
-      </c>
-      <c r="F53" t="s">
-        <v>475</v>
-      </c>
-      <c r="G53" t="s">
-        <v>476</v>
-      </c>
-      <c r="H53" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B54" s="35">
         <v>40</v>
@@ -3720,24 +3723,24 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E54" t="s">
+        <v>475</v>
+      </c>
+      <c r="F54" t="s">
+        <v>476</v>
+      </c>
+      <c r="G54" t="s">
+        <v>477</v>
+      </c>
+      <c r="H54" t="s">
         <v>478</v>
-      </c>
-      <c r="F54" t="s">
-        <v>479</v>
-      </c>
-      <c r="G54" t="s">
-        <v>480</v>
-      </c>
-      <c r="H54" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B55" s="35">
         <v>41</v>
@@ -3746,16 +3749,16 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E55" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F55" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G55" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3818,7 +3821,7 @@
     </row>
     <row r="58" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B58" s="35" t="s">
         <v>139</v>
@@ -3847,7 +3850,7 @@
     </row>
     <row r="59" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B59" s="35" t="s">
         <v>140</v>
@@ -3876,7 +3879,7 @@
     </row>
     <row r="60" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B60" s="35" t="s">
         <v>141</v>
@@ -3905,7 +3908,7 @@
     </row>
     <row r="61" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B61" s="35" t="s">
         <v>142</v>
@@ -3934,7 +3937,7 @@
     </row>
     <row r="62" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B62" s="35" t="s">
         <v>143</v>
@@ -3963,7 +3966,7 @@
     </row>
     <row r="63" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B63" s="35" t="s">
         <v>144</v>
@@ -3992,7 +3995,7 @@
     </row>
     <row r="64" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B64" s="35" t="s">
         <v>145</v>
@@ -4021,7 +4024,7 @@
     </row>
     <row r="65" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B65" s="35" t="s">
         <v>146</v>
@@ -4050,7 +4053,7 @@
     </row>
     <row r="66" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B66" s="35" t="s">
         <v>147</v>
@@ -4079,7 +4082,7 @@
     </row>
     <row r="67" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B67" s="35" t="s">
         <v>148</v>
@@ -4108,7 +4111,7 @@
     </row>
     <row r="68" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B68" s="35" t="s">
         <v>149</v>
@@ -4137,7 +4140,7 @@
     </row>
     <row r="69" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B69" s="35" t="s">
         <v>150</v>
@@ -4224,7 +4227,7 @@
     </row>
     <row r="72" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B72" s="35" t="s">
         <v>153</v>
@@ -4253,7 +4256,7 @@
     </row>
     <row r="73" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B73" s="35" t="s">
         <v>154</v>
@@ -4282,7 +4285,7 @@
     </row>
     <row r="74" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B74" s="35" t="s">
         <v>155</v>
@@ -4316,7 +4319,7 @@
     </row>
     <row r="76" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B76" s="37">
         <v>51</v>
@@ -4325,33 +4328,33 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
+        <v>360</v>
+      </c>
+      <c r="E76" t="s">
         <v>361</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>362</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>363</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>364</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>365</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>366</v>
       </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>367</v>
-      </c>
-      <c r="K76" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B77" s="37">
         <v>52</v>
@@ -4360,33 +4363,33 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
+        <v>368</v>
+      </c>
+      <c r="E77" t="s">
         <v>369</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>370</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>371</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>372</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>373</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>374</v>
       </c>
-      <c r="J77" t="s">
+      <c r="K77" t="s">
         <v>375</v>
-      </c>
-      <c r="K77" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B78" s="37">
         <v>53</v>
@@ -4395,28 +4398,28 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
+        <v>376</v>
+      </c>
+      <c r="E78" t="s">
         <v>377</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>378</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>379</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>380</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>381</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>382</v>
       </c>
-      <c r="J78" t="s">
+      <c r="K78" t="s">
         <v>383</v>
-      </c>
-      <c r="K78" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4430,37 +4433,37 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
+        <v>384</v>
+      </c>
+      <c r="E79" t="s">
         <v>385</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>386</v>
       </c>
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>387</v>
       </c>
-      <c r="G79" t="s">
-        <v>388</v>
-      </c>
       <c r="H79" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I79" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J79" t="s">
+        <v>394</v>
+      </c>
+      <c r="K79" t="s">
         <v>395</v>
       </c>
-      <c r="K79" t="s">
+      <c r="L79" t="s">
         <v>396</v>
       </c>
-      <c r="L79" t="s">
+      <c r="M79" t="s">
         <v>397</v>
       </c>
-      <c r="M79" t="s">
-        <v>398</v>
-      </c>
       <c r="N79" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4474,34 +4477,34 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
+        <v>388</v>
+      </c>
+      <c r="E80" t="s">
+        <v>402</v>
+      </c>
+      <c r="F80" t="s">
         <v>389</v>
       </c>
-      <c r="E80" t="s">
+      <c r="G80" t="s">
+        <v>390</v>
+      </c>
+      <c r="H80" t="s">
+        <v>400</v>
+      </c>
+      <c r="I80" t="s">
         <v>403</v>
       </c>
-      <c r="F80" t="s">
-        <v>390</v>
-      </c>
-      <c r="G80" t="s">
-        <v>391</v>
-      </c>
-      <c r="H80" t="s">
-        <v>401</v>
-      </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>404</v>
       </c>
-      <c r="J80" t="s">
+      <c r="K80" t="s">
         <v>405</v>
       </c>
-      <c r="K80" t="s">
+      <c r="L80" t="s">
         <v>406</v>
       </c>
-      <c r="L80" t="s">
+      <c r="M80" t="s">
         <v>407</v>
-      </c>
-      <c r="M80" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -4515,39 +4518,39 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
+        <v>391</v>
+      </c>
+      <c r="E81" t="s">
+        <v>408</v>
+      </c>
+      <c r="F81" t="s">
         <v>392</v>
       </c>
-      <c r="E81" t="s">
+      <c r="G81" t="s">
+        <v>393</v>
+      </c>
+      <c r="H81" t="s">
         <v>409</v>
       </c>
-      <c r="F81" t="s">
-        <v>393</v>
-      </c>
-      <c r="G81" t="s">
-        <v>394</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>410</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>411</v>
       </c>
-      <c r="J81" t="s">
+      <c r="K81" t="s">
         <v>412</v>
       </c>
-      <c r="K81" t="s">
+      <c r="L81" t="s">
         <v>413</v>
       </c>
-      <c r="L81" t="s">
+      <c r="M81" t="s">
         <v>414</v>
-      </c>
-      <c r="M81" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B82" s="37">
         <v>57</v>
@@ -4556,27 +4559,27 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
+        <v>415</v>
+      </c>
+      <c r="E82" t="s">
         <v>416</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>417</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>418</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>419</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>420</v>
-      </c>
-      <c r="I82" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B83" s="37">
         <v>58</v>
@@ -4585,21 +4588,21 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
+        <v>421</v>
+      </c>
+      <c r="E83" t="s">
         <v>422</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>423</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G83" t="s">
         <v>424</v>
-      </c>
-      <c r="G83" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B84" s="37">
         <v>59</v>
@@ -4608,31 +4611,31 @@
         <v>0</v>
       </c>
       <c r="D84" t="s">
+        <v>425</v>
+      </c>
+      <c r="E84" t="s">
         <v>426</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>427</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G84" t="s">
         <v>428</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>429</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>430</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
+        <v>432</v>
+      </c>
+      <c r="K84" t="s">
+        <v>433</v>
+      </c>
+      <c r="L84" t="s">
         <v>431</v>
-      </c>
-      <c r="J84" t="s">
-        <v>433</v>
-      </c>
-      <c r="K84" t="s">
-        <v>434</v>
-      </c>
-      <c r="L84" t="s">
-        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4651,8 +4654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CB0F51-E2EC-48BC-9E6F-1BD071E06727}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4684,7 +4687,7 @@
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>41</v>
@@ -4707,7 +4710,7 @@
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>80</v>
@@ -4736,7 +4739,7 @@
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>81</v>
@@ -4794,7 +4797,7 @@
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>83</v>
@@ -4852,7 +4855,7 @@
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>44</v>
@@ -4875,7 +4878,7 @@
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>45</v>
@@ -4927,7 +4930,7 @@
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>47</v>
@@ -4948,10 +4951,10 @@
         <v>159</v>
       </c>
       <c r="H12" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="I12" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="J12" t="s">
         <v>183</v>
@@ -4991,7 +4994,7 @@
     </row>
     <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>85</v>
@@ -5049,7 +5052,7 @@
     </row>
     <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>87</v>
@@ -5200,7 +5203,7 @@
     </row>
     <row r="22" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>69</v>
@@ -5209,10 +5212,10 @@
         <v>60</v>
       </c>
       <c r="D22" t="s">
+        <v>442</v>
+      </c>
+      <c r="E22" t="s">
         <v>443</v>
-      </c>
-      <c r="E22" t="s">
-        <v>444</v>
       </c>
       <c r="F22" t="s">
         <v>185</v>
@@ -5220,7 +5223,7 @@
     </row>
     <row r="23" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>88</v>
@@ -5249,7 +5252,7 @@
     </row>
     <row r="24" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>89</v>
@@ -5336,7 +5339,7 @@
     </row>
     <row r="27" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>92</v>
@@ -5365,7 +5368,7 @@
     </row>
     <row r="28" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>93</v>
@@ -5394,7 +5397,7 @@
     </row>
     <row r="29" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>94</v>
@@ -5423,7 +5426,7 @@
     </row>
     <row r="30" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>95</v>
@@ -5481,7 +5484,7 @@
     </row>
     <row r="32" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>97</v>
@@ -5597,7 +5600,7 @@
     </row>
     <row r="36" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>101</v>
@@ -5684,7 +5687,7 @@
     </row>
     <row r="39" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>70</v>
@@ -5693,21 +5696,21 @@
         <v>60</v>
       </c>
       <c r="D39" t="s">
+        <v>482</v>
+      </c>
+      <c r="E39" t="s">
         <v>485</v>
       </c>
-      <c r="E39" t="s">
-        <v>488</v>
-      </c>
       <c r="F39" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="G39" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B40" s="31" t="s">
         <v>71</v>
@@ -5716,16 +5719,16 @@
         <v>72</v>
       </c>
       <c r="D40" t="s">
+        <v>482</v>
+      </c>
+      <c r="E40" t="s">
         <v>485</v>
       </c>
-      <c r="E40" t="s">
-        <v>488</v>
-      </c>
       <c r="F40" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="G40" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -5997,7 +6000,7 @@
     </row>
     <row r="51" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>113</v>
@@ -6026,7 +6029,7 @@
     </row>
     <row r="52" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B52" s="32" t="s">
         <v>114</v>
@@ -6055,7 +6058,7 @@
     </row>
     <row r="53" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="B53" s="32" t="s">
         <v>115</v>
@@ -6084,7 +6087,7 @@
     </row>
     <row r="54" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="B54" s="32" t="s">
         <v>116</v>
@@ -6461,7 +6464,7 @@
     </row>
     <row r="67" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B67" s="32" t="s">
         <v>73</v>

</xml_diff>